<commit_message>
V3V4 processing gel image
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D0A8F4-FB1C-2E48-BB6D-B6341E86A882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94AAE72-D55F-4B42-AFB8-EB765E5E3A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="520" windowWidth="27980" windowHeight="18880" activeTab="2" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="35080" yWindow="1120" windowWidth="27980" windowHeight="18880" activeTab="2" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -833,7 +833,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B25"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
57C gel with new ladder
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94AAE72-D55F-4B42-AFB8-EB765E5E3A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261F496C-52AB-E64C-9A32-94CE21A38732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35080" yWindow="1120" windowWidth="27980" windowHeight="18880" activeTab="2" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
     <sheet name="PCR settings" sheetId="2" r:id="rId2"/>
-    <sheet name="Test samples" sheetId="3" r:id="rId3"/>
+    <sheet name="Protocol Testing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -336,6 +336,24 @@
   </si>
   <si>
     <t>57 C Test</t>
+  </si>
+  <si>
+    <t>GeneRuler 1kb plus DNA LAdder on 2% gel: 100V, 400amp, 1 hour</t>
+  </si>
+  <si>
+    <t>Gel 1:</t>
+  </si>
+  <si>
+    <t>Gel 2:</t>
+  </si>
+  <si>
+    <t>Above 30 samples from all 3 temps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57C set, with bright band samples diluted and not diluted to see if there are 2 bands </t>
+  </si>
+  <si>
+    <t>GeneRuler 100 bp DNA Ladder on 2% gel: 75V, 400amp, 1 hour</t>
   </si>
 </sst>
 </file>
@@ -478,18 +496,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -499,20 +511,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -846,12 +864,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -911,11 +929,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -943,7 +961,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1009,7 +1027,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="24" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1020,7 +1038,7 @@
       <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1029,7 +1047,7 @@
       <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -1056,10 +1074,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,50 +1093,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="27" t="s">
         <v>72</v>
       </c>
@@ -1134,25 +1152,25 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>2878</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1160,22 +1178,22 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>2513</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>91</v>
       </c>
       <c r="H5" t="s">
@@ -1184,7 +1202,7 @@
       <c r="I5" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1192,22 +1210,22 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>63</v>
       </c>
       <c r="H6" t="s">
@@ -1216,28 +1234,28 @@
       <c r="I6" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="18">
         <v>1</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="18">
         <v>2</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="18">
         <v>3</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="18">
         <v>4</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="18">
         <v>5</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="18">
         <v>6</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="18">
         <v>7</v>
       </c>
-      <c r="R6" s="20">
+      <c r="R6" s="18">
         <v>8</v>
       </c>
     </row>
@@ -1245,22 +1263,22 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>65</v>
       </c>
       <c r="H7" t="s">
@@ -1295,22 +1313,22 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>78</v>
       </c>
       <c r="H8" t="s">
@@ -1345,22 +1363,22 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>79</v>
       </c>
       <c r="H9" t="s">
@@ -1371,28 +1389,28 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>80</v>
       </c>
       <c r="H10" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="18">
         <v>9</v>
       </c>
       <c r="L10" s="7">
@@ -1401,13 +1419,13 @@
       <c r="M10" s="7">
         <v>9</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="18">
         <v>10</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="17">
         <v>10</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="17">
         <v>10</v>
       </c>
     </row>
@@ -1415,22 +1433,22 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>81</v>
       </c>
       <c r="H11" t="s">
@@ -1441,19 +1459,19 @@
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>66</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>62</v>
       </c>
       <c r="G12" t="s">
@@ -1467,54 +1485,54 @@
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K14" s="20">
+      <c r="K14" s="18">
         <v>1</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="18">
         <v>2</v>
       </c>
-      <c r="M14" s="20">
+      <c r="M14" s="18">
         <v>3</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="18">
         <v>4</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="18">
         <v>5</v>
       </c>
-      <c r="P14" s="20">
+      <c r="P14" s="18">
         <v>6</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="Q14" s="18">
         <v>7</v>
       </c>
-      <c r="R14" s="20">
+      <c r="R14" s="18">
         <v>8</v>
       </c>
     </row>
@@ -1545,12 +1563,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
       <c r="K16" s="7">
         <v>1</v>
       </c>
@@ -1597,7 +1615,7 @@
       <c r="C18">
         <v>10</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="18">
         <v>9</v>
       </c>
       <c r="L18" s="7">
@@ -1606,13 +1624,13 @@
       <c r="M18" s="7">
         <v>9</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="18">
         <v>10</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="17">
         <v>10</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="17">
         <v>10</v>
       </c>
     </row>
@@ -1639,36 +1657,36 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="18">
         <v>1</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="18">
         <v>2</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M22" s="18">
         <v>3</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="18">
         <v>4</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="18">
         <v>5</v>
       </c>
-      <c r="P22" s="20">
+      <c r="P22" s="18">
         <v>6</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="18">
         <v>7</v>
       </c>
-      <c r="R22" s="20">
+      <c r="R22" s="18">
         <v>8</v>
       </c>
     </row>
@@ -1699,12 +1717,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
       <c r="K24" s="7">
         <v>1</v>
       </c>
@@ -1737,7 +1755,7 @@
       <c r="C25" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1752,11 +1770,11 @@
         <f>30*3*1.05</f>
         <v>94.5</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <f>B26*C26</f>
         <v>1181.25</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="18">
         <v>9</v>
       </c>
       <c r="L26" s="7">
@@ -1765,13 +1783,13 @@
       <c r="M26" s="7">
         <v>9</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="18">
         <v>10</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="17">
         <v>10</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="17">
         <v>10</v>
       </c>
     </row>
@@ -1786,7 +1804,7 @@
         <f t="shared" ref="C27:C29" si="0">30*3*1.05</f>
         <v>94.5</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="10">
         <f t="shared" ref="D27:D29" si="1">B27*C27</f>
         <v>47.25</v>
       </c>
@@ -1802,7 +1820,7 @@
         <f t="shared" si="0"/>
         <v>94.5</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="10">
         <f t="shared" si="1"/>
         <v>47.25</v>
       </c>
@@ -1818,11 +1836,11 @@
         <f t="shared" si="0"/>
         <v>94.5</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="10">
         <f t="shared" si="1"/>
         <v>992.25</v>
       </c>
-      <c r="K29" s="20"/>
+      <c r="K29" s="18"/>
       <c r="L29" t="s">
         <v>73</v>
       </c>
@@ -1843,6 +1861,32 @@
       </c>
       <c r="E32" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dec july phys processing
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261F496C-52AB-E64C-9A32-94CE21A38732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3865DDF-EE5C-BA46-94CA-E9D19EDC4322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35080" yWindow="1120" windowWidth="27980" windowHeight="18880" activeTab="2" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="6220" yWindow="920" windowWidth="27980" windowHeight="18880" activeTab="2" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
calc post and v3v4 trial#2
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3865DDF-EE5C-BA46-94CA-E9D19EDC4322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5823685D-0D2A-2640-8A9C-DFCF1B759DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="920" windowWidth="27980" windowHeight="18880" activeTab="2" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="5620" yWindow="920" windowWidth="27980" windowHeight="18880" activeTab="3" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
     <sheet name="PCR settings" sheetId="2" r:id="rId2"/>
-    <sheet name="Protocol Testing" sheetId="3" r:id="rId3"/>
+    <sheet name="Testing1" sheetId="3" r:id="rId3"/>
+    <sheet name="Testing2 - 20220404" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="130">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -110,12 +111,6 @@
     <t xml:space="preserve">72 °C       </t>
   </si>
   <si>
-    <t xml:space="preserve">5 min min </t>
-  </si>
-  <si>
-    <t xml:space="preserve">55 °C        </t>
-  </si>
-  <si>
     <t>2 Pacuta, 2 Mcap adults, 2 eggs, 2 settled recruits and 1 negative control and 1 positive control (Kevin's)</t>
   </si>
   <si>
@@ -354,13 +349,91 @@
   </si>
   <si>
     <t>GeneRuler 100 bp DNA Ladder on 2% gel: 75V, 400amp, 1 hour</t>
+  </si>
+  <si>
+    <t>Original DNA tube</t>
+  </si>
+  <si>
+    <t>Vial #10</t>
+  </si>
+  <si>
+    <t>DNA concentration (ng/uL)</t>
+  </si>
+  <si>
+    <t>DNA for dilution (uL)</t>
+  </si>
+  <si>
+    <t>Ultrapure H20 for dilution (uL)</t>
+  </si>
+  <si>
+    <t>in 20 uL dilution volume -- 4 ng/uL*20uL reaction / Qubit value = 80/Qubit value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard DNA boxes </t>
+  </si>
+  <si>
+    <t>KBay DNA box</t>
+  </si>
+  <si>
+    <t>ES-17 (M-212 12-4-2019)</t>
+  </si>
+  <si>
+    <t>ES-16 (M-217 12-4-2019)</t>
+  </si>
+  <si>
+    <t>20190722 Ext ID 65, 66</t>
+  </si>
+  <si>
+    <t>20190807 Ext ID 319, 320</t>
+  </si>
+  <si>
+    <t>20210225 Ext ID 17</t>
+  </si>
+  <si>
+    <t>20210225 Ext ID 16</t>
+  </si>
+  <si>
+    <t>too low</t>
+  </si>
+  <si>
+    <t>pull 3 uL straight from Kevin's dilution</t>
+  </si>
+  <si>
+    <t>Porites july bleaching DNA extracts</t>
+  </si>
+  <si>
+    <t>Duplicates instead of triplicates</t>
+  </si>
+  <si>
+    <t>n=20</t>
+  </si>
+  <si>
+    <t>N (20*2*1.05)</t>
+  </si>
+  <si>
+    <t>58 C Test</t>
+  </si>
+  <si>
+    <t>Strip tubes for 2 trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57 °C        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 min  </t>
+  </si>
+  <si>
+    <t>#6 on 58C is 2 uL of D2 (correct)</t>
+  </si>
+  <si>
+    <t>Notes: #5 on 58C run is 2 uL of D1 and 2 uL of D2 (mix-up)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -427,6 +500,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -442,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -483,11 +570,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -534,6 +630,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,59 +1021,59 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -990,7 +1091,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1134,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>21</v>
@@ -1054,7 +1155,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1076,8 +1177,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,7 +1195,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -1110,35 +1211,35 @@
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
@@ -1156,22 +1257,22 @@
         <v>2878</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1182,28 +1283,28 @@
         <v>2513</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1211,28 +1312,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
@@ -1264,25 +1365,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K7" s="7">
         <v>1</v>
@@ -1314,25 +1415,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K8" s="7">
         <v>1</v>
@@ -1364,25 +1465,25 @@
         <v>6</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1390,25 +1491,25 @@
         <v>7</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="G10" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K10" s="18">
         <v>9</v>
@@ -1434,25 +1535,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1460,25 +1561,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" t="s">
-        <v>68</v>
-      </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1486,28 +1587,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1564,7 +1665,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -1596,13 +1697,13 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1658,12 +1759,12 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K21" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C22" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K22" s="18">
         <v>1</v>
@@ -1718,7 +1819,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -1750,18 +1851,18 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>12.5</v>
@@ -1795,7 +1896,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>0.5</v>
@@ -1811,7 +1912,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28">
         <v>0.5</v>
@@ -1827,7 +1928,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B29">
         <v>10.5</v>
@@ -1842,7 +1943,7 @@
       </c>
       <c r="K29" s="18"/>
       <c r="L29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -1851,7 +1952,7 @@
         <v>2268</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -1860,33 +1961,33 @@
         <v>94.5</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1899,4 +2000,749 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2B5181-9F04-7141-BDC3-07C81E007A08}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="28"/>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15">
+        <v>2878</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="8">
+        <v>48.7</v>
+      </c>
+      <c r="H5" s="30">
+        <f>80/G5</f>
+        <v>1.6427104722792607</v>
+      </c>
+      <c r="I5" s="30">
+        <f>20-H5</f>
+        <v>18.357289527720738</v>
+      </c>
+      <c r="J5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2513</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="8">
+        <v>12.55</v>
+      </c>
+      <c r="H6" s="30">
+        <f>80/G6</f>
+        <v>6.3745019920318722</v>
+      </c>
+      <c r="I6" s="30">
+        <f>20-H6</f>
+        <v>13.625498007968128</v>
+      </c>
+      <c r="J6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="8">
+        <v>32.9</v>
+      </c>
+      <c r="H7" s="30">
+        <f t="shared" ref="H7:H12" si="0">80/G7</f>
+        <v>2.43161094224924</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" ref="I7:I12" si="1">20-H7</f>
+        <v>17.56838905775076</v>
+      </c>
+      <c r="J7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="8">
+        <v>36.5</v>
+      </c>
+      <c r="H8" s="30">
+        <f t="shared" si="0"/>
+        <v>2.1917808219178081</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="1"/>
+        <v>17.80821917808219</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="30" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I9" s="30" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="30" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I10" s="30" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8">
+        <v>31.4</v>
+      </c>
+      <c r="H11" s="30">
+        <f t="shared" si="0"/>
+        <v>2.547770700636943</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="1"/>
+        <v>17.452229299363058</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="8">
+        <v>51</v>
+      </c>
+      <c r="H12" s="30">
+        <f t="shared" si="0"/>
+        <v>1.5686274509803921</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="1"/>
+        <v>18.431372549019606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H13" s="30">
+        <f>80/G13</f>
+        <v>7.8431372549019613</v>
+      </c>
+      <c r="I13" s="30">
+        <f>20-H13</f>
+        <v>12.156862745098039</v>
+      </c>
+      <c r="J13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>57</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>58</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>12.5</v>
+      </c>
+      <c r="C26">
+        <f>20*2*1.05</f>
+        <v>42</v>
+      </c>
+      <c r="D26" s="10">
+        <f>B26*C26</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C29" si="2">20*2*1.05</f>
+        <v>42</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" ref="D27:D29" si="3">B27*C27</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>10.5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="3"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f>SUM(D26:D29)</f>
+        <v>1008</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f>D31/24</f>
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>1</v>
+      </c>
+      <c r="B38" s="18">
+        <v>2</v>
+      </c>
+      <c r="C38" s="18">
+        <v>3</v>
+      </c>
+      <c r="D38" s="18">
+        <v>4</v>
+      </c>
+      <c r="E38" s="18">
+        <v>5</v>
+      </c>
+      <c r="F38" s="18">
+        <v>6</v>
+      </c>
+      <c r="G38" s="18">
+        <v>7</v>
+      </c>
+      <c r="H38" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>1</v>
+      </c>
+      <c r="B39" s="7">
+        <v>2</v>
+      </c>
+      <c r="C39" s="7">
+        <v>3</v>
+      </c>
+      <c r="D39" s="7">
+        <v>4</v>
+      </c>
+      <c r="E39" s="7">
+        <v>5</v>
+      </c>
+      <c r="F39" s="7">
+        <v>6</v>
+      </c>
+      <c r="G39" s="7">
+        <v>7</v>
+      </c>
+      <c r="H39" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
+        <v>9</v>
+      </c>
+      <c r="B41" s="7">
+        <v>9</v>
+      </c>
+      <c r="C41" s="7">
+        <v>9</v>
+      </c>
+      <c r="D41" s="18">
+        <v>10</v>
+      </c>
+      <c r="E41" s="17">
+        <v>10</v>
+      </c>
+      <c r="F41" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>1</v>
+      </c>
+      <c r="B45" s="18">
+        <v>2</v>
+      </c>
+      <c r="C45" s="18">
+        <v>3</v>
+      </c>
+      <c r="D45" s="18">
+        <v>4</v>
+      </c>
+      <c r="E45" s="18">
+        <v>5</v>
+      </c>
+      <c r="F45" s="18">
+        <v>6</v>
+      </c>
+      <c r="G45" s="18">
+        <v>7</v>
+      </c>
+      <c r="H45" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>1</v>
+      </c>
+      <c r="B46" s="7">
+        <v>2</v>
+      </c>
+      <c r="C46" s="7">
+        <v>3</v>
+      </c>
+      <c r="D46" s="7">
+        <v>4</v>
+      </c>
+      <c r="E46" s="7">
+        <v>5</v>
+      </c>
+      <c r="F46" s="7">
+        <v>6</v>
+      </c>
+      <c r="G46" s="7">
+        <v>7</v>
+      </c>
+      <c r="H46" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>9</v>
+      </c>
+      <c r="B48" s="7">
+        <v>9</v>
+      </c>
+      <c r="C48" s="7">
+        <v>9</v>
+      </c>
+      <c r="D48" s="18">
+        <v>10</v>
+      </c>
+      <c r="E48" s="17">
+        <v>10</v>
+      </c>
+      <c r="F48" s="17">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A35:H35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="45" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trial 2 gel image
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5823685D-0D2A-2640-8A9C-DFCF1B759DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D61E526-20E1-4E4A-BC65-124018ED7D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5620" yWindow="920" windowWidth="27980" windowHeight="18880" activeTab="3" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
@@ -2010,7 +2010,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
E5 notebook post, gel images, V3V4 excel sheet
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D61E526-20E1-4E4A-BC65-124018ED7D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FF3BD-E445-7A4E-B466-372274E79CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="920" windowWidth="27980" windowHeight="18880" activeTab="3" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
     <sheet name="PCR settings" sheetId="2" r:id="rId2"/>
     <sheet name="Testing1" sheetId="3" r:id="rId3"/>
     <sheet name="Testing2 - 20220404" sheetId="4" r:id="rId4"/>
+    <sheet name="Testing3 - 20220406" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -427,13 +428,115 @@
   </si>
   <si>
     <t>Notes: #5 on 58C run is 2 uL of D1 and 2 uL of D2 (mix-up)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low and High DNA concentration (ng/uL) Trial with some that had a strong band and some that had a faint band </t>
+  </si>
+  <si>
+    <t>96 well plate</t>
+  </si>
+  <si>
+    <t>(-)</t>
+  </si>
+  <si>
+    <t>SampleID</t>
+  </si>
+  <si>
+    <t>Input concentration</t>
+  </si>
+  <si>
+    <t>P.acuta 2513 adult</t>
+  </si>
+  <si>
+    <t>P. ast KW-10</t>
+  </si>
+  <si>
+    <t>8 ng/uL</t>
+  </si>
+  <si>
+    <t>M. cap D1 eggs</t>
+  </si>
+  <si>
+    <t>M. cap Plug10</t>
+  </si>
+  <si>
+    <t>P. acuta 2878 adult</t>
+  </si>
+  <si>
+    <t>M. cap M-212</t>
+  </si>
+  <si>
+    <t>Bright band</t>
+  </si>
+  <si>
+    <t>No band</t>
+  </si>
+  <si>
+    <t>Faint/No band</t>
+  </si>
+  <si>
+    <t>M. cap M-217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">too low so we have the most we can get for those </t>
+  </si>
+  <si>
+    <t>Labeled plug 10</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Already have the above done from Testing2 - 20220404 tubes</t>
+  </si>
+  <si>
+    <t>in 20 uL dilution volume -- 8 ng/uL*20uL reaction / Qubit value = 160/Qubit value</t>
+  </si>
+  <si>
+    <t>N (12*3*1.05)</t>
+  </si>
+  <si>
+    <t>Thaw:</t>
+  </si>
+  <si>
+    <t>F primer, R primer</t>
+  </si>
+  <si>
+    <t>original DNA extract</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -514,6 +617,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -529,7 +654,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -579,11 +704,156 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -612,6 +882,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,11 +902,67 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,12 +1293,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1030,10 +1358,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1128,7 +1456,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1139,7 +1467,7 @@
       <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1148,7 +1476,7 @@
       <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -1194,20 +1522,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1238,16 +1566,16 @@
         <v>87</v>
       </c>
       <c r="J3" s="12"/>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1664,12 +1992,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="K16" s="7">
         <v>1</v>
       </c>
@@ -1818,12 +2146,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
       <c r="K24" s="7">
         <v>1</v>
       </c>
@@ -2009,8 +2337,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="A24:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2027,35 +2355,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="28"/>
+      <c r="B3" s="22"/>
     </row>
     <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -2111,11 +2439,11 @@
       <c r="G5" s="8">
         <v>48.7</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="23">
         <f>80/G5</f>
         <v>1.6427104722792607</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="23">
         <f>20-H5</f>
         <v>18.357289527720738</v>
       </c>
@@ -2145,11 +2473,11 @@
       <c r="G6" s="8">
         <v>12.55</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="23">
         <f>80/G6</f>
         <v>6.3745019920318722</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="23">
         <f>20-H6</f>
         <v>13.625498007968128</v>
       </c>
@@ -2179,11 +2507,11 @@
       <c r="G7" s="8">
         <v>32.9</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="23">
         <f t="shared" ref="H7:H12" si="0">80/G7</f>
         <v>2.43161094224924</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="23">
         <f t="shared" ref="I7:I12" si="1">20-H7</f>
         <v>17.56838905775076</v>
       </c>
@@ -2213,11 +2541,11 @@
       <c r="G8" s="8">
         <v>36.5</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="23">
         <f t="shared" si="0"/>
         <v>2.1917808219178081</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="23">
         <f t="shared" si="1"/>
         <v>17.80821917808219</v>
       </c>
@@ -2245,11 +2573,11 @@
       <c r="G9" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="30" t="e">
+      <c r="H9" s="23" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I9" s="30" t="e">
+      <c r="I9" s="23" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -2277,11 +2605,11 @@
       <c r="G10" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H10" s="30" t="e">
+      <c r="H10" s="23" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I10" s="30" t="e">
+      <c r="I10" s="23" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -2309,11 +2637,11 @@
       <c r="G11" s="8">
         <v>31.4</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="23">
         <f t="shared" si="0"/>
         <v>2.547770700636943</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="23">
         <f t="shared" si="1"/>
         <v>17.452229299363058</v>
       </c>
@@ -2337,11 +2665,11 @@
       <c r="G12" s="8">
         <v>51</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="23">
         <f t="shared" si="0"/>
         <v>1.5686274509803921</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="23">
         <f t="shared" si="1"/>
         <v>18.431372549019606</v>
       </c>
@@ -2368,11 +2696,11 @@
       <c r="G13">
         <v>10.199999999999999</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="23">
         <f>80/G13</f>
         <v>7.8431372549019613</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="23">
         <f>20-H13</f>
         <v>12.156862745098039</v>
       </c>
@@ -2413,12 +2741,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2468,12 +2796,12 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -2569,16 +2897,16 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
@@ -2745,4 +3073,907 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE27BFF9-8F67-5C4E-8759-EF333DAAF436}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>4</v>
+      </c>
+      <c r="F4" s="6">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>6</v>
+      </c>
+      <c r="H4" s="6">
+        <v>7</v>
+      </c>
+      <c r="I4" s="6">
+        <v>8</v>
+      </c>
+      <c r="J4" s="6">
+        <v>9</v>
+      </c>
+      <c r="K4" s="6">
+        <v>10</v>
+      </c>
+      <c r="L4" s="6">
+        <v>11</v>
+      </c>
+      <c r="M4" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="18">
+        <v>7</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7</v>
+      </c>
+      <c r="H5" s="7">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="18">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7">
+        <v>8</v>
+      </c>
+      <c r="H6" s="7">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="18">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="18">
+        <v>9</v>
+      </c>
+      <c r="G7" s="7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="7">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="18">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="18">
+        <v>10</v>
+      </c>
+      <c r="G8" s="7">
+        <v>10</v>
+      </c>
+      <c r="H8" s="7">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="35">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="18">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7">
+        <v>11</v>
+      </c>
+      <c r="H9" s="7">
+        <v>11</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="36">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="18">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7">
+        <v>12</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+    </row>
+    <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="39">
+        <v>1</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="51">
+        <v>12.55</v>
+      </c>
+      <c r="G17" s="52">
+        <f>80/F17</f>
+        <v>6.3745019920318722</v>
+      </c>
+      <c r="H17" s="53">
+        <f>20-G17</f>
+        <v>13.625498007968128</v>
+      </c>
+      <c r="I17" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="39">
+        <v>2</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" s="41">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G18" s="56">
+        <f t="shared" ref="G18:G22" si="0">80/F18</f>
+        <v>7.8431372549019613</v>
+      </c>
+      <c r="H18" s="57">
+        <f t="shared" ref="H18:H22" si="1">20-G18</f>
+        <v>12.156862745098039</v>
+      </c>
+      <c r="I18" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="39">
+        <v>3</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="55">
+        <v>31.4</v>
+      </c>
+      <c r="G19" s="56">
+        <f t="shared" si="0"/>
+        <v>2.547770700636943</v>
+      </c>
+      <c r="H19" s="57">
+        <f t="shared" si="1"/>
+        <v>17.452229299363058</v>
+      </c>
+      <c r="I19" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="39">
+        <v>4</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="55">
+        <v>48.7</v>
+      </c>
+      <c r="G20" s="56">
+        <f t="shared" si="0"/>
+        <v>1.6427104722792607</v>
+      </c>
+      <c r="H20" s="57">
+        <f t="shared" si="1"/>
+        <v>18.357289527720738</v>
+      </c>
+      <c r="I20" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="39">
+        <v>5</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="55">
+        <v>36.5</v>
+      </c>
+      <c r="G21" s="56">
+        <f t="shared" si="0"/>
+        <v>2.1917808219178081</v>
+      </c>
+      <c r="H21" s="57">
+        <f t="shared" si="1"/>
+        <v>17.80821917808219</v>
+      </c>
+      <c r="I21" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+    </row>
+    <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39">
+        <v>6</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="63">
+        <v>32.9</v>
+      </c>
+      <c r="G22" s="58">
+        <f t="shared" si="0"/>
+        <v>2.43161094224924</v>
+      </c>
+      <c r="H22" s="59">
+        <f t="shared" si="1"/>
+        <v>17.56838905775076</v>
+      </c>
+      <c r="I22" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="39">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="55">
+        <v>12.55</v>
+      </c>
+      <c r="G23" s="56">
+        <f>160/F23</f>
+        <v>12.749003984063744</v>
+      </c>
+      <c r="H23" s="57">
+        <f>20-G23</f>
+        <v>7.2509960159362556</v>
+      </c>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="39">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" s="41">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G24" s="56">
+        <f t="shared" ref="G24:G28" si="2">160/F24</f>
+        <v>15.686274509803923</v>
+      </c>
+      <c r="H24" s="57">
+        <f t="shared" ref="H24:H28" si="3">20-G24</f>
+        <v>4.3137254901960773</v>
+      </c>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="39">
+        <v>9</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="55">
+        <v>31.4</v>
+      </c>
+      <c r="G25" s="56">
+        <f t="shared" si="2"/>
+        <v>5.095541401273886</v>
+      </c>
+      <c r="H25" s="57">
+        <f t="shared" si="3"/>
+        <v>14.904458598726114</v>
+      </c>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="39">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="55">
+        <v>48.7</v>
+      </c>
+      <c r="G26" s="56">
+        <f t="shared" si="2"/>
+        <v>3.2854209445585214</v>
+      </c>
+      <c r="H26" s="57">
+        <f t="shared" si="3"/>
+        <v>16.714579055441479</v>
+      </c>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="39">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="55">
+        <v>36.5</v>
+      </c>
+      <c r="G27" s="56">
+        <f t="shared" si="2"/>
+        <v>4.3835616438356162</v>
+      </c>
+      <c r="H27" s="57">
+        <f t="shared" si="3"/>
+        <v>15.616438356164384</v>
+      </c>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="39">
+        <v>12</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="62">
+        <v>32.9</v>
+      </c>
+      <c r="G28" s="60">
+        <f t="shared" si="2"/>
+        <v>4.86322188449848</v>
+      </c>
+      <c r="H28" s="61">
+        <f t="shared" si="3"/>
+        <v>15.136778115501521</v>
+      </c>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="34"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="F37" s="71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>12.5</v>
+      </c>
+      <c r="C39">
+        <f>12*3*1.05</f>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="D39" s="10">
+        <f>B39*C39</f>
+        <v>472.50000000000006</v>
+      </c>
+      <c r="F39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40">
+        <v>0.5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40:C42" si="4">12*3*1.05</f>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="D40" s="10">
+        <f t="shared" ref="D40:D42" si="5">B40*C40</f>
+        <v>18.900000000000002</v>
+      </c>
+      <c r="F40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41">
+        <v>0.5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="4"/>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="D41" s="10">
+        <f t="shared" si="5"/>
+        <v>18.900000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42">
+        <v>10.5</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="4"/>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="D42" s="10">
+        <f t="shared" si="5"/>
+        <v>396.90000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <f>SUM(D39:D42)</f>
+        <v>907.2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <f>D44/24</f>
+        <v>37.800000000000004</v>
+      </c>
+      <c r="E45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
+  </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
primer info and v3v4 sample processing
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FF3BD-E445-7A4E-B466-372274E79CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7D6A40-3634-8E48-823D-36287A6ECAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="5" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
     <sheet name="PCR settings" sheetId="2" r:id="rId2"/>
-    <sheet name="Testing1" sheetId="3" r:id="rId3"/>
+    <sheet name="Testing1 - 20220321" sheetId="3" r:id="rId3"/>
     <sheet name="Testing2 - 20220404" sheetId="4" r:id="rId4"/>
     <sheet name="Testing3 - 20220406" sheetId="5" r:id="rId5"/>
+    <sheet name="Sequencing URI GSC 1" sheetId="7" r:id="rId6"/>
+    <sheet name="Sequencing sheet for Janet 1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="206">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -67,9 +69,6 @@
     <t>806RB reverse</t>
   </si>
   <si>
-    <t xml:space="preserve">388F forward </t>
-  </si>
-  <si>
     <t>ACTCCTACGGGAGGCAGCA</t>
   </si>
   <si>
@@ -530,13 +529,142 @@
   </si>
   <si>
     <t>original DNA extract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">338F forward </t>
+  </si>
+  <si>
+    <t>Sending samples for a test sequencing run with Janet at URI GSC</t>
+  </si>
+  <si>
+    <t>Date PCR run</t>
+  </si>
+  <si>
+    <t>**too low**</t>
+  </si>
+  <si>
+    <t>Band information</t>
+  </si>
+  <si>
+    <t>faint</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>DNA input</t>
+  </si>
+  <si>
+    <t>8 ng/uL (24 ng total)</t>
+  </si>
+  <si>
+    <t>Pocillopora acuta</t>
+  </si>
+  <si>
+    <t>Porites asteroides</t>
+  </si>
+  <si>
+    <t>Montipora capitata</t>
+  </si>
+  <si>
+    <t>Lifestage</t>
+  </si>
+  <si>
+    <t>Settled recruit</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>KW-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug10 </t>
+  </si>
+  <si>
+    <t>M-217</t>
+  </si>
+  <si>
+    <t>M-212</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>ELS001</t>
+  </si>
+  <si>
+    <t>ELS002</t>
+  </si>
+  <si>
+    <t>ELS003</t>
+  </si>
+  <si>
+    <t>ELS004</t>
+  </si>
+  <si>
+    <t>ELS005</t>
+  </si>
+  <si>
+    <t>ELS006</t>
+  </si>
+  <si>
+    <t>ELS007</t>
+  </si>
+  <si>
+    <t>ELS008</t>
+  </si>
+  <si>
+    <t>Strip tube # to Janet</t>
+  </si>
+  <si>
+    <t>Original strip tube #</t>
+  </si>
+  <si>
+    <t>Strip Tube #</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>16S</t>
+  </si>
+  <si>
+    <t>25 uL of sample to URI GSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uL leftover after </t>
+  </si>
+  <si>
+    <t>3 (70 uL)</t>
+  </si>
+  <si>
+    <t>Replicate # (uL total after gel)</t>
+  </si>
+  <si>
+    <t>2 (45 uL)</t>
+  </si>
+  <si>
+    <t>20 uL</t>
+  </si>
+  <si>
+    <t>45 uL</t>
+  </si>
+  <si>
+    <t>4 ng/uL (12 ng total)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -635,6 +763,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -853,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -884,6 +1026,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -908,41 +1085,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -961,8 +1106,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,7 +1444,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,12 +1457,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1321,16 +1485,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1341,67 +1505,68 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="25"/>
+      <c r="A14" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="60"/>
       <c r="C14" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="C24" s="58"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1429,21 +1594,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -1451,39 +1616,39 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="61" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="26"/>
+        <v>20</v>
+      </c>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="26"/>
+        <v>21</v>
+      </c>
+      <c r="C5" s="61"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1506,7 +1671,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1522,60 +1687,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="I3" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J3" s="12"/>
-      <c r="K3" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
+      <c r="K3" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1585,22 +1750,22 @@
         <v>2878</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1611,28 +1776,28 @@
         <v>2513</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
         <v>89</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>90</v>
-      </c>
       <c r="K5" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1640,28 +1805,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
@@ -1693,25 +1858,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="7">
         <v>1</v>
@@ -1743,25 +1908,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="7">
         <v>1</v>
@@ -1793,25 +1958,25 @@
         <v>6</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1819,25 +1984,25 @@
         <v>7</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="18">
         <v>9</v>
@@ -1863,25 +2028,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1889,25 +2054,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1915,28 +2080,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1992,12 +2157,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="A16" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
       <c r="K16" s="7">
         <v>1</v>
       </c>
@@ -2025,13 +2190,13 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -2087,12 +2252,12 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K21" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C22" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K22" s="18">
         <v>1</v>
@@ -2146,12 +2311,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="A24" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
       <c r="K24" s="7">
         <v>1</v>
       </c>
@@ -2179,18 +2344,18 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26">
         <v>12.5</v>
@@ -2224,7 +2389,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>0.5</v>
@@ -2240,7 +2405,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>0.5</v>
@@ -2256,7 +2421,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>10.5</v>
@@ -2271,7 +2436,7 @@
       </c>
       <c r="K29" s="18"/>
       <c r="L29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -2280,7 +2445,7 @@
         <v>2268</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -2289,33 +2454,33 @@
         <v>94.5</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2338,7 +2503,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="A24:E32"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2355,66 +2520,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="B2" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="22"/>
     </row>
     <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>108</v>
-      </c>
       <c r="J4" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -2425,16 +2590,16 @@
         <v>2878</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G5" s="8">
         <v>48.7</v>
@@ -2448,7 +2613,7 @@
         <v>18.357289527720738</v>
       </c>
       <c r="J5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2459,16 +2624,16 @@
         <v>2513</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="8">
         <v>12.55</v>
@@ -2482,7 +2647,7 @@
         <v>13.625498007968128</v>
       </c>
       <c r="J6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -2490,19 +2655,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="8">
         <v>32.9</v>
@@ -2516,7 +2681,7 @@
         <v>17.56838905775076</v>
       </c>
       <c r="J7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -2524,19 +2689,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="F8" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G8" s="8">
         <v>36.5</v>
@@ -2550,7 +2715,7 @@
         <v>17.80821917808219</v>
       </c>
       <c r="J8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -2558,20 +2723,20 @@
         <v>5</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H9" s="23" t="e">
         <f t="shared" si="0"/>
@@ -2582,7 +2747,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -2590,20 +2755,20 @@
         <v>6</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H10" s="23" t="e">
         <f t="shared" si="0"/>
@@ -2614,7 +2779,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -2622,16 +2787,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8">
@@ -2651,16 +2816,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="8">
         <v>51</v>
@@ -2679,19 +2844,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="F13" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G13">
         <v>10.199999999999999</v>
@@ -2705,7 +2870,7 @@
         <v>12.156862745098039</v>
       </c>
       <c r="J13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -2713,53 +2878,53 @@
         <v>10</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="A17" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2773,7 +2938,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2787,36 +2952,36 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="A24" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26">
         <v>12.5</v>
@@ -2832,7 +2997,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>0.5</v>
@@ -2848,7 +3013,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>0.5</v>
@@ -2864,7 +3029,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>10.5</v>
@@ -2884,7 +3049,7 @@
         <v>1008</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2893,24 +3058,24 @@
         <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
+      <c r="A35" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -2987,7 +3152,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -3082,8 +3247,8 @@
   </sheetPr>
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3101,27 +3266,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
+      <c r="A1" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -3165,7 +3330,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="18">
         <v>1</v>
@@ -3188,7 +3353,7 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -3196,7 +3361,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="18">
         <v>2</v>
@@ -3219,7 +3384,7 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -3227,7 +3392,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" s="18">
         <v>3</v>
@@ -3250,7 +3415,7 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -3258,7 +3423,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="18">
         <v>4</v>
@@ -3287,9 +3452,9 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="35">
+        <v>133</v>
+      </c>
+      <c r="B9" s="27">
         <v>5</v>
       </c>
       <c r="C9" s="7">
@@ -3316,9 +3481,9 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="36">
+        <v>134</v>
+      </c>
+      <c r="B10" s="28">
         <v>6</v>
       </c>
       <c r="C10" s="7">
@@ -3344,11 +3509,11 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>136</v>
+      <c r="A11" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="32"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -3362,9 +3527,9 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="33"/>
+        <v>136</v>
+      </c>
+      <c r="B12" s="25"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -3379,7 +3544,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -3395,489 +3560,489 @@
       <c r="M13" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>104</v>
+      <c r="D16" s="39" t="s">
+        <v>103</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="H16" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="39">
+      <c r="A17" s="31">
         <v>1</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="F17" s="51">
+      <c r="B17" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F17" s="42">
         <v>12.55</v>
       </c>
-      <c r="G17" s="52">
+      <c r="G17" s="43">
         <f>80/F17</f>
         <v>6.3745019920318722</v>
       </c>
-      <c r="H17" s="53">
+      <c r="H17" s="44">
         <f>20-G17</f>
         <v>13.625498007968128</v>
       </c>
-      <c r="I17" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
+      <c r="I17" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="39">
+      <c r="A18" s="31">
         <v>2</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="F18" s="41">
+      <c r="B18" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="33">
         <v>10.199999999999999</v>
       </c>
-      <c r="G18" s="56">
+      <c r="G18" s="47">
         <f t="shared" ref="G18:G22" si="0">80/F18</f>
         <v>7.8431372549019613</v>
       </c>
-      <c r="H18" s="57">
+      <c r="H18" s="48">
         <f t="shared" ref="H18:H22" si="1">20-G18</f>
         <v>12.156862745098039</v>
       </c>
-      <c r="I18" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
+      <c r="I18" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="39">
+      <c r="A19" s="31">
         <v>3</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" s="55">
+      <c r="B19" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="46">
         <v>31.4</v>
       </c>
-      <c r="G19" s="56">
+      <c r="G19" s="47">
         <f t="shared" si="0"/>
         <v>2.547770700636943</v>
       </c>
-      <c r="H19" s="57">
+      <c r="H19" s="48">
         <f t="shared" si="1"/>
         <v>17.452229299363058</v>
       </c>
-      <c r="I19" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
+      <c r="I19" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="39">
+      <c r="A20" s="31">
         <v>4</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="55">
+      <c r="B20" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="46">
         <v>48.7</v>
       </c>
-      <c r="G20" s="56">
+      <c r="G20" s="47">
         <f t="shared" si="0"/>
         <v>1.6427104722792607</v>
       </c>
-      <c r="H20" s="57">
+      <c r="H20" s="48">
         <f t="shared" si="1"/>
         <v>18.357289527720738</v>
       </c>
-      <c r="I20" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
+      <c r="I20" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="39">
+      <c r="A21" s="31">
         <v>5</v>
       </c>
-      <c r="B21" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="F21" s="55">
+      <c r="B21" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="46">
         <v>36.5</v>
       </c>
-      <c r="G21" s="56">
+      <c r="G21" s="47">
         <f t="shared" si="0"/>
         <v>2.1917808219178081</v>
       </c>
-      <c r="H21" s="57">
+      <c r="H21" s="48">
         <f t="shared" si="1"/>
         <v>17.80821917808219</v>
       </c>
-      <c r="I21" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
+      <c r="I21" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="31">
         <v>6</v>
       </c>
-      <c r="B22" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="F22" s="63">
+      <c r="B22" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="54">
         <v>32.9</v>
       </c>
-      <c r="G22" s="58">
+      <c r="G22" s="49">
         <f t="shared" si="0"/>
         <v>2.43161094224924</v>
       </c>
-      <c r="H22" s="59">
+      <c r="H22" s="50">
         <f t="shared" si="1"/>
         <v>17.56838905775076</v>
       </c>
-      <c r="I22" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+      <c r="I22" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="39">
+      <c r="A23" s="31">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E23" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" s="55">
+        <v>150</v>
+      </c>
+      <c r="F23" s="46">
         <v>12.55</v>
       </c>
-      <c r="G23" s="56">
+      <c r="G23" s="47">
         <f>160/F23</f>
         <v>12.749003984063744</v>
       </c>
-      <c r="H23" s="57">
+      <c r="H23" s="48">
         <f>20-G23</f>
         <v>7.2509960159362556</v>
       </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="39">
+      <c r="A24" s="31">
         <v>8</v>
       </c>
       <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" t="s">
         <v>145</v>
       </c>
-      <c r="C24" t="s">
-        <v>146</v>
-      </c>
       <c r="D24" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="41">
+        <v>150</v>
+      </c>
+      <c r="F24" s="33">
         <v>10.199999999999999</v>
       </c>
-      <c r="G24" s="56">
+      <c r="G24" s="47">
         <f t="shared" ref="G24:G28" si="2">160/F24</f>
         <v>15.686274509803923</v>
       </c>
-      <c r="H24" s="57">
+      <c r="H24" s="48">
         <f t="shared" ref="H24:H28" si="3">20-G24</f>
         <v>4.3137254901960773</v>
       </c>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="39">
+      <c r="A25" s="31">
         <v>9</v>
       </c>
-      <c r="B25" s="34" t="s">
-        <v>148</v>
+      <c r="B25" s="26" t="s">
+        <v>147</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="55">
+        <v>152</v>
+      </c>
+      <c r="F25" s="46">
         <v>31.4</v>
       </c>
-      <c r="G25" s="56">
+      <c r="G25" s="47">
         <f t="shared" si="2"/>
         <v>5.095541401273886</v>
       </c>
-      <c r="H25" s="57">
+      <c r="H25" s="48">
         <f t="shared" si="3"/>
         <v>14.904458598726114</v>
       </c>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="39">
+      <c r="A26" s="31">
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F26" s="55">
+        <v>152</v>
+      </c>
+      <c r="F26" s="46">
         <v>48.7</v>
       </c>
-      <c r="G26" s="56">
+      <c r="G26" s="47">
         <f t="shared" si="2"/>
         <v>3.2854209445585214</v>
       </c>
-      <c r="H26" s="57">
+      <c r="H26" s="48">
         <f t="shared" si="3"/>
         <v>16.714579055441479</v>
       </c>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="39">
+      <c r="A27" s="31">
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F27" s="55">
+        <v>151</v>
+      </c>
+      <c r="F27" s="46">
         <v>36.5</v>
       </c>
-      <c r="G27" s="56">
+      <c r="G27" s="47">
         <f t="shared" si="2"/>
         <v>4.3835616438356162</v>
       </c>
-      <c r="H27" s="57">
+      <c r="H27" s="48">
         <f t="shared" si="3"/>
         <v>15.616438356164384</v>
       </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="39">
+      <c r="A28" s="31">
         <v>12</v>
       </c>
-      <c r="B28" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="F28" s="62">
+      <c r="B28" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="53">
         <v>32.9</v>
       </c>
-      <c r="G28" s="60">
+      <c r="G28" s="51">
         <f t="shared" si="2"/>
         <v>4.86322188449848</v>
       </c>
-      <c r="H28" s="61">
+      <c r="H28" s="52">
         <f t="shared" si="3"/>
         <v>15.136778115501521</v>
       </c>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>157</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>147</v>
+        <v>156</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>146</v>
       </c>
       <c r="C30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="67"/>
+      <c r="B33" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="68" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="70"/>
+      <c r="B34" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="73"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="34"/>
+      <c r="C35" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="F37" s="71" t="s">
-        <v>161</v>
+      <c r="A37" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="F37" s="56" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C38" t="s">
-        <v>160</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="F38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39">
         <v>12.5</v>
@@ -3891,12 +4056,12 @@
         <v>472.50000000000006</v>
       </c>
       <c r="F39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40">
         <v>0.5</v>
@@ -3910,12 +4075,12 @@
         <v>18.900000000000002</v>
       </c>
       <c r="F40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>0.5</v>
@@ -3931,7 +4096,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42">
         <v>10.5</v>
@@ -3951,7 +4116,7 @@
         <v>907.2</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3960,7 +4125,7 @@
         <v>37.800000000000004</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3976,4 +4141,528 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E45E1A-AD6F-5D47-B9F5-6F99D46DA9AE}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="75" customWidth="1"/>
+    <col min="2" max="2" width="20" style="75" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="75" customWidth="1"/>
+    <col min="4" max="6" width="19.83203125" style="75" customWidth="1"/>
+    <col min="7" max="7" width="22" style="75" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="75" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="75"/>
+    <col min="10" max="10" width="16.83203125" style="75" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+    </row>
+    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="75">
+        <v>1</v>
+      </c>
+      <c r="C5" s="77">
+        <v>7</v>
+      </c>
+      <c r="D5" s="75">
+        <v>2513</v>
+      </c>
+      <c r="E5" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="75">
+        <v>20220406</v>
+      </c>
+      <c r="I5" s="75">
+        <v>3</v>
+      </c>
+      <c r="J5" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="K5" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L5" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="75">
+        <v>2</v>
+      </c>
+      <c r="C6" s="77">
+        <v>8</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="75">
+        <v>20220406</v>
+      </c>
+      <c r="I6" s="75">
+        <v>3</v>
+      </c>
+      <c r="J6" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L6" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="75">
+        <v>3</v>
+      </c>
+      <c r="C7" s="77">
+        <v>9</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="75">
+        <v>20220406</v>
+      </c>
+      <c r="I7" s="75">
+        <v>3</v>
+      </c>
+      <c r="J7" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="K7" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L7" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="75">
+        <v>4</v>
+      </c>
+      <c r="C8" s="77">
+        <v>10</v>
+      </c>
+      <c r="D8" s="75">
+        <v>2878</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="78" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="75" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" s="75">
+        <v>20220321</v>
+      </c>
+      <c r="I8" s="75">
+        <v>1</v>
+      </c>
+      <c r="J8" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="K8" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L8" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="75" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="75">
+        <v>5</v>
+      </c>
+      <c r="C9" s="77">
+        <v>11</v>
+      </c>
+      <c r="D9" s="75" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9" s="75">
+        <v>20220406</v>
+      </c>
+      <c r="I9" s="75">
+        <v>3</v>
+      </c>
+      <c r="J9" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="K9" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L9" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="75" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="75">
+        <v>6</v>
+      </c>
+      <c r="C10" s="77">
+        <v>12</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="H10" s="75">
+        <v>20220406</v>
+      </c>
+      <c r="I10" s="75">
+        <v>3</v>
+      </c>
+      <c r="J10" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L10" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="75" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="75">
+        <v>7</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="75">
+        <v>20220406</v>
+      </c>
+      <c r="I11" s="75">
+        <v>3</v>
+      </c>
+      <c r="J11" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="K11" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="L11" s="75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="75">
+        <v>8</v>
+      </c>
+      <c r="C12" s="75">
+        <v>5</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="H12" s="75">
+        <v>20220404</v>
+      </c>
+      <c r="I12" s="75">
+        <v>2</v>
+      </c>
+      <c r="J12" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="K12" s="75" t="s">
+        <v>202</v>
+      </c>
+      <c r="L12" s="75" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68591B-911E-1D4D-A731-F1CC3E4BE9FA}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="75">
+        <v>1</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="75">
+        <v>2</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="75"/>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="75">
+        <v>3</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="75"/>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="75">
+        <v>4</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="75"/>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="75">
+        <v>5</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="75"/>
+      <c r="D6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="75">
+        <v>6</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="75">
+        <v>7</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="75">
+        <v>8</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="75"/>
+      <c r="D9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
16S 541F primer sequence to be ordered and E5 calc updates
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7D6A40-3634-8E48-823D-36287A6ECAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD74B64-309F-AA4C-8BBE-4869D3EB0CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="5" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="211">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -658,13 +658,28 @@
   </si>
   <si>
     <t>4 ng/uL (12 ng total)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>341F forward</t>
+  </si>
+  <si>
+    <t>CCTACGGGNGGCWGCAG</t>
+  </si>
+  <si>
+    <t>TCGTCGGCAGCGTCAGATGTGTATAAGAGACAGCCTACGGGNGGCWGCAG</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -689,18 +704,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF2E2E2E"/>
-      <name val="Georgia"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF24292F"/>
-      <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
@@ -780,6 +783,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -995,21 +1025,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1022,10 +1050,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1033,21 +1064,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1058,55 +1089,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1121,10 +1149,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1441,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DB150A-2BCE-B84B-8778-606C9E17DCA4}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1456,20 +1490,20 @@
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1482,97 +1516,136 @@
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="57" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="E6" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="C8" s="80"/>
+      <c r="D8" s="81"/>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="C9" s="79"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="82"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+    <row r="17" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="B17" s="22"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="C24" s="57"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="58"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1593,64 +1666,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="59" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="61"/>
+      <c r="C4" s="59"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="59"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1687,84 +1760,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="64" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>2878</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1772,22 +1845,22 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>2513</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>88</v>
       </c>
       <c r="H5" t="s">
@@ -1796,7 +1869,7 @@
       <c r="I5" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1804,22 +1877,22 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>60</v>
       </c>
       <c r="H6" t="s">
@@ -1828,28 +1901,28 @@
       <c r="I6" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="16">
         <v>1</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="16">
         <v>2</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="16">
         <v>3</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="16">
         <v>4</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="16">
         <v>5</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="16">
         <v>6</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="Q6" s="16">
         <v>7</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="16">
         <v>8</v>
       </c>
     </row>
@@ -1857,49 +1930,49 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>62</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="5">
         <v>1</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="5">
         <v>2</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="5">
         <v>3</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="5">
         <v>4</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="5">
         <v>5</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="5">
         <v>6</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="5">
         <v>7</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1907,49 +1980,49 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>75</v>
       </c>
       <c r="H8" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="5">
         <v>1</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="5">
         <v>2</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="5">
         <v>3</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="5">
         <v>4</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="5">
         <v>5</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="5">
         <v>6</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="5">
         <v>7</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1957,22 +2030,22 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>76</v>
       </c>
       <c r="H9" t="s">
@@ -1983,43 +2056,43 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="6" t="s">
         <v>77</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="16">
         <v>9</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="5">
         <v>9</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="5">
         <v>9</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="16">
         <v>10</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="15">
         <v>10</v>
       </c>
-      <c r="P10" s="17">
+      <c r="P10" s="15">
         <v>10</v>
       </c>
     </row>
@@ -2027,22 +2100,22 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>78</v>
       </c>
       <c r="H11" t="s">
@@ -2053,19 +2126,19 @@
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G12" t="s">
@@ -2079,112 +2152,112 @@
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K14" s="18">
+      <c r="K14" s="16">
         <v>1</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="16">
         <v>2</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="16">
         <v>3</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="16">
         <v>4</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="16">
         <v>5</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="16">
         <v>6</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q14" s="16">
         <v>7</v>
       </c>
-      <c r="R14" s="18">
+      <c r="R14" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K15" s="7">
+      <c r="K15" s="5">
         <v>1</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="5">
         <v>2</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="5">
         <v>3</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="5">
         <v>4</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="5">
         <v>5</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="5">
         <v>6</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="5">
         <v>7</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="K16" s="7">
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="K16" s="5">
         <v>1</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="5">
         <v>2</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="5">
         <v>3</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="5">
         <v>4</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="5">
         <v>5</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="5">
         <v>6</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="5">
         <v>7</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="5">
         <v>8</v>
       </c>
     </row>
@@ -2209,22 +2282,22 @@
       <c r="C18">
         <v>10</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="16">
         <v>9</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="5">
         <v>9</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="5">
         <v>9</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="16">
         <v>10</v>
       </c>
-      <c r="O18" s="17">
+      <c r="O18" s="15">
         <v>10</v>
       </c>
-      <c r="P18" s="17">
+      <c r="P18" s="15">
         <v>10</v>
       </c>
     </row>
@@ -2251,94 +2324,94 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="16">
         <v>1</v>
       </c>
-      <c r="L22" s="18">
+      <c r="L22" s="16">
         <v>2</v>
       </c>
-      <c r="M22" s="18">
+      <c r="M22" s="16">
         <v>3</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="16">
         <v>4</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22" s="16">
         <v>5</v>
       </c>
-      <c r="P22" s="18">
+      <c r="P22" s="16">
         <v>6</v>
       </c>
-      <c r="Q22" s="18">
+      <c r="Q22" s="16">
         <v>7</v>
       </c>
-      <c r="R22" s="18">
+      <c r="R22" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K23" s="7">
+      <c r="K23" s="5">
         <v>1</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="5">
         <v>2</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="5">
         <v>3</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="5">
         <v>4</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="5">
         <v>5</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="5">
         <v>6</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="Q23" s="5">
         <v>7</v>
       </c>
-      <c r="R23" s="7">
+      <c r="R23" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="K24" s="7">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="K24" s="5">
         <v>1</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="5">
         <v>2</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="5">
         <v>3</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="5">
         <v>4</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="5">
         <v>5</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="5">
         <v>6</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q24" s="5">
         <v>7</v>
       </c>
-      <c r="R24" s="7">
+      <c r="R24" s="5">
         <v>8</v>
       </c>
     </row>
@@ -2349,7 +2422,7 @@
       <c r="C25" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2364,26 +2437,26 @@
         <f>30*3*1.05</f>
         <v>94.5</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="8">
         <f>B26*C26</f>
         <v>1181.25</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="16">
         <v>9</v>
       </c>
-      <c r="L26" s="7">
+      <c r="L26" s="5">
         <v>9</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="5">
         <v>9</v>
       </c>
-      <c r="N26" s="18">
+      <c r="N26" s="16">
         <v>10</v>
       </c>
-      <c r="O26" s="17">
+      <c r="O26" s="15">
         <v>10</v>
       </c>
-      <c r="P26" s="17">
+      <c r="P26" s="15">
         <v>10</v>
       </c>
     </row>
@@ -2398,7 +2471,7 @@
         <f t="shared" ref="C27:C29" si="0">30*3*1.05</f>
         <v>94.5</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="8">
         <f t="shared" ref="D27:D29" si="1">B27*C27</f>
         <v>47.25</v>
       </c>
@@ -2414,7 +2487,7 @@
         <f t="shared" si="0"/>
         <v>94.5</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="8">
         <f t="shared" si="1"/>
         <v>47.25</v>
       </c>
@@ -2430,11 +2503,11 @@
         <f t="shared" si="0"/>
         <v>94.5</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="8">
         <f t="shared" si="1"/>
         <v>992.25</v>
       </c>
-      <c r="K29" s="18"/>
+      <c r="K29" s="16"/>
       <c r="L29" t="s">
         <v>70</v>
       </c>
@@ -2520,65 +2593,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="22"/>
+      <c r="B3" s="20"/>
     </row>
     <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2586,29 +2659,29 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="13">
         <v>2878</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>48.7</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="21">
         <f>80/G5</f>
         <v>1.6427104722792607</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="21">
         <f>20-H5</f>
         <v>18.357289527720738</v>
       </c>
@@ -2620,29 +2693,29 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>2513</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>12.55</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="21">
         <f>80/G6</f>
         <v>6.3745019920318722</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="21">
         <f>20-H6</f>
         <v>13.625498007968128</v>
       </c>
@@ -2654,29 +2727,29 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>32.9</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="21">
         <f t="shared" ref="H7:H12" si="0">80/G7</f>
         <v>2.43161094224924</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="21">
         <f t="shared" ref="I7:I12" si="1">20-H7</f>
         <v>17.56838905775076</v>
       </c>
@@ -2688,29 +2761,29 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>36.5</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="21">
         <f t="shared" si="0"/>
         <v>2.1917808219178081</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="21">
         <f t="shared" si="1"/>
         <v>17.80821917808219</v>
       </c>
@@ -2722,31 +2795,31 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="23" t="e">
+      <c r="H9" s="21" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I9" s="23" t="e">
+      <c r="I9" s="21" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2754,31 +2827,31 @@
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H10" s="23" t="e">
+      <c r="H10" s="21" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I10" s="23" t="e">
+      <c r="I10" s="21" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="6" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2786,27 +2859,27 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
         <v>31.4</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="21">
         <f t="shared" si="0"/>
         <v>2.547770700636943</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="21">
         <f t="shared" si="1"/>
         <v>17.452229299363058</v>
       </c>
@@ -2815,26 +2888,26 @@
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>51</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
         <f t="shared" si="0"/>
         <v>1.5686274509803921</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="21">
         <f t="shared" si="1"/>
         <v>18.431372549019606</v>
       </c>
@@ -2843,29 +2916,29 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>104</v>
       </c>
       <c r="G13">
         <v>10.199999999999999</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="21">
         <f>80/G13</f>
         <v>7.8431372549019613</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="21">
         <f>20-H13</f>
         <v>12.156862745098039</v>
       </c>
@@ -2877,41 +2950,41 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2956,17 +3029,17 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -2975,7 +3048,7 @@
       <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2990,7 +3063,7 @@
         <f>20*2*1.05</f>
         <v>42</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="8">
         <f>B26*C26</f>
         <v>525</v>
       </c>
@@ -3006,7 +3079,7 @@
         <f t="shared" ref="C27:C29" si="2">20*2*1.05</f>
         <v>42</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="8">
         <f t="shared" ref="D27:D29" si="3">B27*C27</f>
         <v>21</v>
       </c>
@@ -3022,7 +3095,7 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="8">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
@@ -3038,7 +3111,7 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="8">
         <f t="shared" si="3"/>
         <v>441</v>
       </c>
@@ -3062,168 +3135,168 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="18">
+      <c r="A38" s="16">
         <v>1</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="16">
         <v>2</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="16">
         <v>3</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D38" s="16">
         <v>4</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="16">
         <v>5</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="16">
         <v>6</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="16">
         <v>7</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H38" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
+      <c r="A39" s="5">
         <v>1</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="5">
         <v>2</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="5">
         <v>3</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="5">
         <v>4</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="5">
         <v>5</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="5">
         <v>6</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="5">
         <v>7</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="18">
+      <c r="A41" s="16">
         <v>9</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="5">
         <v>9</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="5">
         <v>9</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D41" s="16">
         <v>10</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="15">
         <v>10</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="18">
+      <c r="A45" s="16">
         <v>1</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="16">
         <v>2</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="16">
         <v>3</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="16">
         <v>4</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="16">
         <v>5</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="16">
         <v>6</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="16">
         <v>7</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
+      <c r="A46" s="5">
         <v>1</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="5">
         <v>2</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="5">
         <v>3</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="5">
         <v>4</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="5">
         <v>5</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="5">
         <v>6</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="5">
         <v>7</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="18">
+      <c r="A48" s="16">
         <v>9</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="5">
         <v>9</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="5">
         <v>9</v>
       </c>
-      <c r="D48" s="18">
+      <c r="D48" s="16">
         <v>10</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="15">
         <v>10</v>
       </c>
-      <c r="F48" s="17">
+      <c r="F48" s="15">
         <v>10</v>
       </c>
     </row>
@@ -3266,23 +3339,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3290,509 +3363,509 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>4</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>6</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>7</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>8</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>9</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="4">
         <v>10</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="4">
         <v>11</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="4">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="18">
+      <c r="E5" s="5"/>
+      <c r="F5" s="16">
         <v>7</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>7</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>7</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="18">
+      <c r="E6" s="5"/>
+      <c r="F6" s="16">
         <v>8</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>8</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>8</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="18">
+      <c r="E7" s="5"/>
+      <c r="F7" s="16">
         <v>9</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>9</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>9</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>4</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>4</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="18">
+      <c r="E8" s="5"/>
+      <c r="F8" s="16">
         <v>10</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>10</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>10</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>5</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>5</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="18">
+      <c r="E9" s="5"/>
+      <c r="F9" s="16">
         <v>11</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>11</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>11</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>6</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>6</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>6</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="18">
+      <c r="E10" s="5"/>
+      <c r="F10" s="16">
         <v>12</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>12</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>12</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="31">
+      <c r="A17" s="30">
         <v>1</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="41">
         <v>12.55</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="42">
         <f>80/F17</f>
         <v>6.3745019920318722</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="43">
         <f>20-G17</f>
         <v>13.625498007968128</v>
       </c>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="31">
+      <c r="A18" s="30">
         <v>2</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <v>10.199999999999999</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="46">
         <f t="shared" ref="G18:G22" si="0">80/F18</f>
         <v>7.8431372549019613</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="47">
         <f t="shared" ref="H18:H22" si="1">20-G18</f>
         <v>12.156862745098039</v>
       </c>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="31">
+      <c r="A19" s="30">
         <v>3</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="45">
         <v>31.4</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="46">
         <f t="shared" si="0"/>
         <v>2.547770700636943</v>
       </c>
-      <c r="H19" s="48">
+      <c r="H19" s="47">
         <f t="shared" si="1"/>
         <v>17.452229299363058</v>
       </c>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="31">
+      <c r="A20" s="30">
         <v>4</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="45">
         <v>48.7</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="46">
         <f t="shared" si="0"/>
         <v>1.6427104722792607</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H20" s="47">
         <f t="shared" si="1"/>
         <v>18.357289527720738</v>
       </c>
-      <c r="I20" s="41" t="s">
+      <c r="I20" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="31">
+      <c r="A21" s="30">
         <v>5</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="F21" s="46">
+      <c r="F21" s="45">
         <v>36.5</v>
       </c>
-      <c r="G21" s="47">
+      <c r="G21" s="46">
         <f t="shared" si="0"/>
         <v>2.1917808219178081</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="47">
         <f t="shared" si="1"/>
         <v>17.80821917808219</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
     </row>
     <row r="22" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31">
+      <c r="A22" s="30">
         <v>6</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="54">
+      <c r="F22" s="53">
         <v>32.9</v>
       </c>
-      <c r="G22" s="49">
+      <c r="G22" s="48">
         <f t="shared" si="0"/>
         <v>2.43161094224924</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="49">
         <f t="shared" si="1"/>
         <v>17.56838905775076</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="31">
+      <c r="A23" s="30">
         <v>7</v>
       </c>
       <c r="B23" t="s">
@@ -3801,29 +3874,29 @@
       <c r="C23" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>113</v>
       </c>
       <c r="E23" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="46">
+      <c r="F23" s="45">
         <v>12.55</v>
       </c>
-      <c r="G23" s="47">
+      <c r="G23" s="46">
         <f>160/F23</f>
         <v>12.749003984063744</v>
       </c>
-      <c r="H23" s="48">
+      <c r="H23" s="47">
         <f>20-G23</f>
         <v>7.2509960159362556</v>
       </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="31">
+      <c r="A24" s="30">
         <v>8</v>
       </c>
       <c r="B24" t="s">
@@ -3832,60 +3905,60 @@
       <c r="C24" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>104</v>
       </c>
       <c r="E24" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="32">
         <v>10.199999999999999</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G24" s="46">
         <f t="shared" ref="G24:G28" si="2">160/F24</f>
         <v>15.686274509803923</v>
       </c>
-      <c r="H24" s="48">
+      <c r="H24" s="47">
         <f t="shared" ref="H24:H28" si="3">20-G24</f>
         <v>4.3137254901960773</v>
       </c>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="31">
+      <c r="A25" s="30">
         <v>9</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C25" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F25" s="46">
+      <c r="F25" s="45">
         <v>31.4</v>
       </c>
-      <c r="G25" s="47">
+      <c r="G25" s="46">
         <f t="shared" si="2"/>
         <v>5.095541401273886</v>
       </c>
-      <c r="H25" s="48">
+      <c r="H25" s="47">
         <f t="shared" si="3"/>
         <v>14.904458598726114</v>
       </c>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="31">
+      <c r="A26" s="30">
         <v>10</v>
       </c>
       <c r="B26" t="s">
@@ -3894,29 +3967,29 @@
       <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="46">
+      <c r="F26" s="45">
         <v>48.7</v>
       </c>
-      <c r="G26" s="47">
+      <c r="G26" s="46">
         <f t="shared" si="2"/>
         <v>3.2854209445585214</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="47">
         <f t="shared" si="3"/>
         <v>16.714579055441479</v>
       </c>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="31">
+      <c r="A27" s="30">
         <v>11</v>
       </c>
       <c r="B27" t="s">
@@ -3925,63 +3998,63 @@
       <c r="C27" t="s">
         <v>145</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="F27" s="46">
+      <c r="F27" s="45">
         <v>36.5</v>
       </c>
-      <c r="G27" s="47">
+      <c r="G27" s="46">
         <f t="shared" si="2"/>
         <v>4.3835616438356162</v>
       </c>
-      <c r="H27" s="48">
+      <c r="H27" s="47">
         <f t="shared" si="3"/>
         <v>15.616438356164384</v>
       </c>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="31">
+      <c r="A28" s="30">
         <v>12</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="F28" s="53">
+      <c r="F28" s="52">
         <v>32.9</v>
       </c>
-      <c r="G28" s="51">
+      <c r="G28" s="50">
         <f t="shared" si="2"/>
         <v>4.86322188449848</v>
       </c>
-      <c r="H28" s="52">
+      <c r="H28" s="51">
         <f t="shared" si="3"/>
         <v>15.136778115501521</v>
       </c>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>146</v>
       </c>
       <c r="C30" t="s">
@@ -3989,40 +4062,40 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="70"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="73"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="71"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="26"/>
+      <c r="C35" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="F37" s="56" t="s">
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="F37" s="55" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4033,7 +4106,7 @@
       <c r="C38" t="s">
         <v>159</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="8" t="s">
         <v>54</v>
       </c>
       <c r="F38" t="s">
@@ -4051,7 +4124,7 @@
         <f>12*3*1.05</f>
         <v>37.800000000000004</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="8">
         <f>B39*C39</f>
         <v>472.50000000000006</v>
       </c>
@@ -4070,7 +4143,7 @@
         <f t="shared" ref="C40:C42" si="4">12*3*1.05</f>
         <v>37.800000000000004</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="8">
         <f t="shared" ref="D40:D42" si="5">B40*C40</f>
         <v>18.900000000000002</v>
       </c>
@@ -4089,7 +4162,7 @@
         <f t="shared" si="4"/>
         <v>37.800000000000004</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="8">
         <f t="shared" si="5"/>
         <v>18.900000000000002</v>
       </c>
@@ -4105,7 +4178,7 @@
         <f t="shared" si="4"/>
         <v>37.800000000000004</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="8">
         <f t="shared" si="5"/>
         <v>396.90000000000003</v>
       </c>
@@ -4137,7 +4210,7 @@
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="B34:I34"/>
   </mergeCells>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4145,396 +4218,401 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E45E1A-AD6F-5D47-B9F5-6F99D46DA9AE}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="75" customWidth="1"/>
-    <col min="2" max="2" width="20" style="75" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="75" customWidth="1"/>
-    <col min="4" max="6" width="19.83203125" style="75" customWidth="1"/>
-    <col min="7" max="7" width="22" style="75" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="75" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="75"/>
-    <col min="10" max="10" width="16.83203125" style="75" customWidth="1"/>
-    <col min="11" max="11" width="26.1640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="73" customWidth="1"/>
+    <col min="2" max="2" width="20" style="73" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="73" customWidth="1"/>
+    <col min="4" max="6" width="19.83203125" style="73" customWidth="1"/>
+    <col min="7" max="7" width="22" style="73" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="73" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="73"/>
+    <col min="10" max="10" width="16.83203125" style="73" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="73" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
     </row>
     <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="77" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="74" t="s">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="72" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="74" t="s">
+      <c r="G4" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="74" t="s">
+      <c r="H4" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="74" t="s">
+      <c r="J4" s="72" t="s">
         <v>167</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="73" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="73">
         <v>1</v>
       </c>
-      <c r="C5" s="77">
+      <c r="C5" s="75">
         <v>7</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="73">
         <v>2513</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="H5" s="75">
+      <c r="H5" s="73">
         <v>20220406</v>
       </c>
-      <c r="I5" s="75">
+      <c r="I5" s="73">
         <v>3</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="73" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="75">
+      <c r="B6" s="73">
         <v>2</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="75">
         <v>8</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="73">
         <v>20220406</v>
       </c>
-      <c r="I6" s="75">
+      <c r="I6" s="73">
         <v>3</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="K6" s="75" t="s">
+      <c r="K6" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L6" s="75" t="s">
+      <c r="L6" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="73" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="73">
         <v>3</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="75">
         <v>9</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="H7" s="75">
+      <c r="H7" s="73">
         <v>20220406</v>
       </c>
-      <c r="I7" s="75">
+      <c r="I7" s="73">
         <v>3</v>
       </c>
-      <c r="J7" s="75" t="s">
+      <c r="J7" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="K7" s="75" t="s">
+      <c r="K7" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L7" s="75" t="s">
+      <c r="L7" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="73" t="s">
         <v>187</v>
       </c>
-      <c r="B8" s="75">
+      <c r="B8" s="73">
         <v>4</v>
       </c>
-      <c r="C8" s="77">
+      <c r="C8" s="75">
         <v>10</v>
       </c>
-      <c r="D8" s="75">
+      <c r="D8" s="73">
         <v>2878</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="75">
+      <c r="H8" s="73">
         <v>20220321</v>
       </c>
-      <c r="I8" s="75">
+      <c r="I8" s="73">
         <v>1</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="75">
+      <c r="B9" s="73">
         <v>5</v>
       </c>
-      <c r="C9" s="77">
+      <c r="C9" s="75">
         <v>11</v>
       </c>
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="73" t="s">
         <v>181</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="78" t="s">
+      <c r="F9" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="G9" s="75" t="s">
+      <c r="G9" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="H9" s="75">
+      <c r="H9" s="73">
         <v>20220406</v>
       </c>
-      <c r="I9" s="75">
+      <c r="I9" s="73">
         <v>3</v>
       </c>
-      <c r="J9" s="75" t="s">
+      <c r="J9" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="K9" s="75" t="s">
+      <c r="K9" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L9" s="75" t="s">
+      <c r="L9" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="B10" s="75">
+      <c r="B10" s="73">
         <v>6</v>
       </c>
-      <c r="C10" s="77">
+      <c r="C10" s="75">
         <v>12</v>
       </c>
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="74" t="s">
         <v>182</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="78" t="s">
+      <c r="F10" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="H10" s="75">
+      <c r="H10" s="73">
         <v>20220406</v>
       </c>
-      <c r="I10" s="75">
+      <c r="I10" s="73">
         <v>3</v>
       </c>
-      <c r="J10" s="75" t="s">
+      <c r="J10" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="K10" s="75" t="s">
+      <c r="K10" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L10" s="75" t="s">
+      <c r="L10" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="75">
+      <c r="B11" s="73">
         <v>7</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="78" t="s">
+      <c r="G11" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="75">
+      <c r="H11" s="73">
         <v>20220406</v>
       </c>
-      <c r="I11" s="75">
+      <c r="I11" s="73">
         <v>3</v>
       </c>
-      <c r="J11" s="75" t="s">
+      <c r="J11" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="L11" s="75" t="s">
+      <c r="L11" s="73" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="73" t="s">
         <v>191</v>
       </c>
-      <c r="B12" s="75">
+      <c r="B12" s="73">
         <v>8</v>
       </c>
-      <c r="C12" s="75">
+      <c r="C12" s="73">
         <v>5</v>
       </c>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="E12" s="78" t="s">
+      <c r="E12" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="G12" s="78" t="s">
+      <c r="G12" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="H12" s="75">
+      <c r="H12" s="73">
         <v>20220404</v>
       </c>
-      <c r="I12" s="75">
+      <c r="I12" s="73">
         <v>2</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="K12" s="75" t="s">
+      <c r="K12" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="L12" s="75" t="s">
+      <c r="L12" s="73" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="73" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:N1"/>
   </mergeCells>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4567,97 +4645,97 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="75">
+      <c r="A2" s="73">
         <v>1</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="73" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="75"/>
+      <c r="C2" s="73"/>
       <c r="D2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="75">
+      <c r="A3" s="73">
         <v>2</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="73"/>
       <c r="D3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="75">
+      <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="73"/>
       <c r="D4" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="75">
+      <c r="A5" s="73">
         <v>4</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="75"/>
+      <c r="C5" s="73"/>
       <c r="D5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="75">
+      <c r="A6" s="73">
         <v>5</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="75"/>
+      <c r="C6" s="73"/>
       <c r="D6" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="75">
+      <c r="A7" s="73">
         <v>6</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="75"/>
+      <c r="C7" s="73"/>
       <c r="D7" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="75">
+      <c r="A8" s="73">
         <v>7</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="73"/>
       <c r="D8" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="75">
+      <c r="A9" s="73">
         <v>8</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="73" t="s">
         <v>191</v>
       </c>
-      <c r="C9" s="75"/>
+      <c r="C9" s="73"/>
       <c r="D9" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
v3v4 excel doc and processing notebook post
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD74B64-309F-AA4C-8BBE-4869D3EB0CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B3C8BF-671A-FC45-80C6-3CEE9E985FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="5" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
     <sheet name="PCR settings" sheetId="2" r:id="rId2"/>
-    <sheet name="Testing1 - 20220321" sheetId="3" r:id="rId3"/>
-    <sheet name="Testing2 - 20220404" sheetId="4" r:id="rId4"/>
-    <sheet name="Testing3 - 20220406" sheetId="5" r:id="rId5"/>
-    <sheet name="Sequencing URI GSC 1" sheetId="7" r:id="rId6"/>
-    <sheet name="Sequencing sheet for Janet 1" sheetId="8" r:id="rId7"/>
+    <sheet name="Testing1 (338F) - 20220321" sheetId="3" r:id="rId3"/>
+    <sheet name="Testing2 (338F) - 20220404" sheetId="4" r:id="rId4"/>
+    <sheet name="Testing3 (338F) - 20220406" sheetId="5" r:id="rId5"/>
+    <sheet name="Testing4 (341F) - 20220413" sheetId="9" r:id="rId6"/>
+    <sheet name="Sequencing URI GSC 1" sheetId="7" r:id="rId7"/>
+    <sheet name="Sequencing sheet for Janet 1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="246">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -294,9 +295,6 @@
     <t>X = 20 uL</t>
   </si>
   <si>
-    <t xml:space="preserve">20 uL 200 uM </t>
-  </si>
-  <si>
     <t>180 uL Ultra Pure water</t>
   </si>
   <si>
@@ -673,6 +671,114 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">341F forward </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resuspending concenrate to 100 uM = started with 58.4 nM so IDT sheet said to add 584 uL to create 100 uM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 uL 100 uM </t>
+  </si>
+  <si>
+    <t>D1 eggs</t>
+  </si>
+  <si>
+    <t>PCR strip tube #</t>
+  </si>
+  <si>
+    <t>KW 4ng/uL plate 1</t>
+  </si>
+  <si>
+    <t>DNA location</t>
+  </si>
+  <si>
+    <t>20220406 8 ng/uL dilution strip tube</t>
+  </si>
+  <si>
+    <t>KW 4ng/uL plate 1 well E7</t>
+  </si>
+  <si>
+    <t>20220406 8 ng/uL dilution strip tube (tube 7)</t>
+  </si>
+  <si>
+    <t>20220406 8 ng/uL dilution strip tube (tube 10)</t>
+  </si>
+  <si>
+    <t>20220406 8 ng/uL dilution strip tube (tube 11)</t>
+  </si>
+  <si>
+    <t>20220406 8 ng/uL dilution strip tube (tube 12)</t>
+  </si>
+  <si>
+    <t>Result from 338F trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">341F primer trial - testing #4 </t>
+  </si>
+  <si>
+    <t>20220406 8 ng/uL dilution strip tube (tube 9)</t>
+  </si>
+  <si>
+    <t>M. cap Plug4</t>
+  </si>
+  <si>
+    <t>DNA (uL)</t>
+  </si>
+  <si>
+    <t>Qubit concentration</t>
+  </si>
+  <si>
+    <t>H20 (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labeled Plug4 in AH's freezer box </t>
+  </si>
+  <si>
+    <t>D2 eggs</t>
+  </si>
+  <si>
+    <t>KW 4ng/uL plate 1 well F7</t>
+  </si>
+  <si>
+    <t>1. Resuspend primer (add 584 uL)</t>
+  </si>
+  <si>
+    <t>2. Make 10 uM primer tube (20 uL of stock + 180 uL of UP H2O)</t>
+  </si>
+  <si>
+    <t>3. Make Plug 4's 8 ng/uL dilution tube</t>
+  </si>
+  <si>
+    <t>PROTOCOL FOR TODAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grab reagents to thaw </t>
+  </si>
+  <si>
+    <t>4. Make master mix solution</t>
+  </si>
+  <si>
+    <t>10 samples * 3 for triplicates * 1.05 for error</t>
+  </si>
+  <si>
+    <t>N (10*3*1.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug 4 tube </t>
+  </si>
+  <si>
+    <t>8 ng/uL dilution strip tube from 20220406</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>25 uL</t>
+  </si>
+  <si>
+    <t>å</t>
   </si>
 </sst>
 </file>
@@ -826,7 +932,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1021,11 +1127,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1092,7 +1224,31 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1134,33 +1290,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1475,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DB150A-2BCE-B84B-8778-606C9E17DCA4}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,12 +1629,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1517,12 +1655,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1556,43 +1694,43 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="E7" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="C8" s="80"/>
-      <c r="D8" s="81"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66"/>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="C9" s="79"/>
+      <c r="C9" s="64"/>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
-        <v>163</v>
-      </c>
-      <c r="B13" s="82"/>
+      <c r="A13" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="68"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1603,7 +1741,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1634,18 +1772,81 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="68" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" s="68"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="22"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1694,18 +1895,18 @@
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="69" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="69"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1714,14 +1915,14 @@
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="59"/>
+      <c r="C5" s="69"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1744,7 +1945,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1760,20 +1961,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1801,19 +2002,19 @@
         <v>32</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1835,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>33</v>
@@ -1861,16 +2062,16 @@
         <v>30</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1899,7 +2100,7 @@
         <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K6" s="16">
         <v>1</v>
@@ -2174,7 +2375,7 @@
         <v>43</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -2230,12 +2431,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
       <c r="K16" s="5">
         <v>1</v>
       </c>
@@ -2325,7 +2526,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K21" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -2384,12 +2585,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
       <c r="K24" s="5">
         <v>1</v>
       </c>
@@ -2532,28 +2733,28 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2576,7 +2777,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2593,32 +2794,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="B2" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
@@ -2640,19 +2841,19 @@
         <v>26</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="J4" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -2672,7 +2873,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="6">
         <v>48.7</v>
@@ -2686,7 +2887,7 @@
         <v>18.357289527720738</v>
       </c>
       <c r="J5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2706,7 +2907,7 @@
         <v>27</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="6">
         <v>12.55</v>
@@ -2720,7 +2921,7 @@
         <v>13.625498007968128</v>
       </c>
       <c r="J6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -2728,7 +2929,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>34</v>
@@ -2740,7 +2941,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="6">
         <v>32.9</v>
@@ -2754,7 +2955,7 @@
         <v>17.56838905775076</v>
       </c>
       <c r="J7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -2762,7 +2963,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>34</v>
@@ -2774,7 +2975,7 @@
         <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" s="6">
         <v>36.5</v>
@@ -2788,7 +2989,7 @@
         <v>17.80821917808219</v>
       </c>
       <c r="J8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -2809,7 +3010,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H9" s="21" t="e">
         <f t="shared" si="0"/>
@@ -2820,7 +3021,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -2841,7 +3042,7 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H10" s="21" t="e">
         <f t="shared" si="0"/>
@@ -2852,7 +3053,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -2929,7 +3130,7 @@
         <v>64</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13">
         <v>10.199999999999999</v>
@@ -2943,7 +3144,7 @@
         <v>12.156862745098039</v>
       </c>
       <c r="J13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -2979,12 +3180,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2997,7 +3198,7 @@
         <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3011,7 +3212,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3025,28 +3226,28 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>54</v>
@@ -3135,20 +3336,20 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="62" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
+      <c r="A35" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -3225,7 +3426,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -3321,7 +3522,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A37" sqref="A37:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3339,17 +3540,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="A1" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -3359,7 +3560,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -3403,7 +3604,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="16">
         <v>1</v>
@@ -3426,7 +3627,7 @@
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -3434,7 +3635,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="16">
         <v>2</v>
@@ -3457,7 +3658,7 @@
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -3465,7 +3666,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="16">
         <v>3</v>
@@ -3488,7 +3689,7 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -3496,7 +3697,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="16">
         <v>4</v>
@@ -3525,7 +3726,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="26">
         <v>5</v>
@@ -3554,7 +3755,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="27">
         <v>6</v>
@@ -3583,7 +3784,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="23"/>
@@ -3600,7 +3801,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="5"/>
@@ -3617,7 +3818,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3633,34 +3834,34 @@
       <c r="M13" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>142</v>
-      </c>
       <c r="D16" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -3671,16 +3872,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F17" s="41">
         <v>12.55</v>
@@ -3694,7 +3895,7 @@
         <v>13.625498007968128</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
@@ -3704,16 +3905,16 @@
         <v>2</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F18" s="32">
         <v>10.199999999999999</v>
@@ -3727,7 +3928,7 @@
         <v>12.156862745098039</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
@@ -3737,16 +3938,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F19" s="45">
         <v>31.4</v>
@@ -3760,7 +3961,7 @@
         <v>17.452229299363058</v>
       </c>
       <c r="I19" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
@@ -3770,16 +3971,16 @@
         <v>4</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" s="45">
         <v>48.7</v>
@@ -3793,7 +3994,7 @@
         <v>18.357289527720738</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
@@ -3803,16 +4004,16 @@
         <v>5</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F21" s="45">
         <v>36.5</v>
@@ -3826,7 +4027,7 @@
         <v>17.80821917808219</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
@@ -3836,16 +4037,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F22" s="53">
         <v>32.9</v>
@@ -3859,7 +4060,7 @@
         <v>17.56838905775076</v>
       </c>
       <c r="I22" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
@@ -3869,16 +4070,16 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F23" s="45">
         <v>12.55</v>
@@ -3900,16 +4101,16 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
         <v>144</v>
       </c>
-      <c r="C24" t="s">
-        <v>145</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F24" s="32">
         <v>10.199999999999999</v>
@@ -3931,16 +4132,16 @@
         <v>9</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F25" s="45">
         <v>31.4</v>
@@ -3962,16 +4163,16 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F26" s="45">
         <v>48.7</v>
@@ -3993,16 +4194,16 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F27" s="45">
         <v>36.5</v>
@@ -4024,16 +4225,16 @@
         <v>12</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E28" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F28" s="52">
         <v>32.9</v>
@@ -4052,51 +4253,51 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="68"/>
+      <c r="B33" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="78"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="71"/>
+      <c r="B34" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="81"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
       <c r="F37" s="55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -4104,7 +4305,7 @@
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>54</v>
@@ -4129,7 +4330,7 @@
         <v>472.50000000000006</v>
       </c>
       <c r="F39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -4148,7 +4349,7 @@
         <v>18.900000000000002</v>
       </c>
       <c r="F40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -4217,395 +4418,831 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB297DE-4901-EF42-A30A-80FA25326886}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="49.5" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="82" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="86" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="85" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="6">
+        <v>51</v>
+      </c>
+      <c r="G10" s="87">
+        <f>160/F10</f>
+        <v>3.1372549019607843</v>
+      </c>
+      <c r="H10" s="88">
+        <f>20-G10</f>
+        <v>16.862745098039216</v>
+      </c>
+      <c r="L10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="85" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="83" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="55" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>235</v>
+      </c>
+      <c r="B21" s="83"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="F27" s="55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>12.5</v>
+      </c>
+      <c r="C29">
+        <f>10*3*1.05</f>
+        <v>31.5</v>
+      </c>
+      <c r="D29" s="8">
+        <f>B29*C29</f>
+        <v>393.75</v>
+      </c>
+      <c r="F29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <v>0.5</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:C32" si="0">10*3*1.05</f>
+        <v>31.5</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" ref="D30:D32" si="1">B30*C30</f>
+        <v>15.75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>31.5</v>
+      </c>
+      <c r="D31" s="8">
+        <f t="shared" si="1"/>
+        <v>15.75</v>
+      </c>
+      <c r="G31" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32">
+        <v>10.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>31.5</v>
+      </c>
+      <c r="D32" s="8">
+        <f t="shared" si="1"/>
+        <v>330.75</v>
+      </c>
+      <c r="G32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f>SUM(D29:D32)</f>
+        <v>756</v>
+      </c>
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f>D34/24</f>
+        <v>31.5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E45E1A-AD6F-5D47-B9F5-6F99D46DA9AE}">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="73" customWidth="1"/>
-    <col min="2" max="2" width="20" style="73" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="73" customWidth="1"/>
-    <col min="4" max="6" width="19.83203125" style="73" customWidth="1"/>
-    <col min="7" max="7" width="22" style="73" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="73" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="73"/>
-    <col min="10" max="10" width="16.83203125" style="73" customWidth="1"/>
-    <col min="11" max="11" width="26.1640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="59" customWidth="1"/>
+    <col min="2" max="2" width="20" style="59" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="59" customWidth="1"/>
+    <col min="4" max="6" width="19.83203125" style="59" customWidth="1"/>
+    <col min="7" max="7" width="22" style="59" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="59" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="59"/>
+    <col min="10" max="10" width="16.83203125" style="59" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="59" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+    </row>
+    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-    </row>
-    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="I4" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="K4" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="72" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="72" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="59">
+        <v>1</v>
+      </c>
+      <c r="C5" s="61">
+        <v>7</v>
+      </c>
+      <c r="D5" s="59">
+        <v>2513</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" s="59">
+        <v>20220406</v>
+      </c>
+      <c r="I5" s="59">
+        <v>3</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="59">
+        <v>2</v>
+      </c>
+      <c r="C6" s="61">
+        <v>8</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" s="59">
+        <v>20220406</v>
+      </c>
+      <c r="I6" s="59">
+        <v>3</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="59">
+        <v>3</v>
+      </c>
+      <c r="C7" s="61">
+        <v>9</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="E7" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="72" t="s">
+      <c r="F7" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="72" t="s">
+      <c r="H7" s="59">
+        <v>20220406</v>
+      </c>
+      <c r="I7" s="59">
+        <v>3</v>
+      </c>
+      <c r="J7" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L7" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="59">
+        <v>4</v>
+      </c>
+      <c r="C8" s="61">
+        <v>10</v>
+      </c>
+      <c r="D8" s="59">
+        <v>2878</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="59">
+        <v>20220321</v>
+      </c>
+      <c r="I8" s="59">
+        <v>1</v>
+      </c>
+      <c r="J8" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="K8" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="59">
+        <v>5</v>
+      </c>
+      <c r="C9" s="61">
+        <v>11</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" s="59">
+        <v>20220406</v>
+      </c>
+      <c r="I9" s="59">
+        <v>3</v>
+      </c>
+      <c r="J9" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="K9" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L9" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="59">
+        <v>6</v>
+      </c>
+      <c r="C10" s="61">
+        <v>12</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="H10" s="59">
+        <v>20220406</v>
+      </c>
+      <c r="I10" s="59">
+        <v>3</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="K10" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L10" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" s="59">
+        <v>7</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="59">
+        <v>20220406</v>
+      </c>
+      <c r="I11" s="59">
+        <v>3</v>
+      </c>
+      <c r="J11" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="K11" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="L11" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="59">
+        <v>8</v>
+      </c>
+      <c r="C12" s="59">
+        <v>5</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="72" t="s">
+      <c r="H12" s="59">
+        <v>20220404</v>
+      </c>
+      <c r="I12" s="59">
+        <v>2</v>
+      </c>
+      <c r="J12" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="K4" s="72" t="s">
+      <c r="K12" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="73" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="73">
-        <v>1</v>
-      </c>
-      <c r="C5" s="75">
-        <v>7</v>
-      </c>
-      <c r="D5" s="73">
-        <v>2513</v>
-      </c>
-      <c r="E5" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="G5" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" s="73">
-        <v>20220406</v>
-      </c>
-      <c r="I5" s="73">
-        <v>3</v>
-      </c>
-      <c r="J5" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="K5" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L5" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" s="73">
-        <v>2</v>
-      </c>
-      <c r="C6" s="75">
-        <v>8</v>
-      </c>
-      <c r="D6" s="73" t="s">
-        <v>179</v>
-      </c>
-      <c r="E6" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="73" t="s">
-        <v>174</v>
-      </c>
-      <c r="G6" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="H6" s="73">
-        <v>20220406</v>
-      </c>
-      <c r="I6" s="73">
-        <v>3</v>
-      </c>
-      <c r="J6" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="K6" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L6" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="B7" s="73">
-        <v>3</v>
-      </c>
-      <c r="C7" s="75">
-        <v>9</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>180</v>
-      </c>
-      <c r="E7" s="74" t="s">
-        <v>177</v>
-      </c>
-      <c r="F7" s="74" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="73">
-        <v>20220406</v>
-      </c>
-      <c r="I7" s="73">
-        <v>3</v>
-      </c>
-      <c r="J7" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="K7" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L7" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="B8" s="73">
-        <v>4</v>
-      </c>
-      <c r="C8" s="75">
-        <v>10</v>
-      </c>
-      <c r="D8" s="73">
-        <v>2878</v>
-      </c>
-      <c r="E8" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="76" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" s="73" t="s">
+      <c r="L12" s="59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="59" t="s">
         <v>205</v>
-      </c>
-      <c r="H8" s="73">
-        <v>20220321</v>
-      </c>
-      <c r="I8" s="73">
-        <v>1</v>
-      </c>
-      <c r="J8" s="73" t="s">
-        <v>168</v>
-      </c>
-      <c r="K8" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L8" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="B9" s="73">
-        <v>5</v>
-      </c>
-      <c r="C9" s="75">
-        <v>11</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>181</v>
-      </c>
-      <c r="E9" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="76" t="s">
-        <v>175</v>
-      </c>
-      <c r="G9" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="H9" s="73">
-        <v>20220406</v>
-      </c>
-      <c r="I9" s="73">
-        <v>3</v>
-      </c>
-      <c r="J9" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="K9" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L9" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="B10" s="73">
-        <v>6</v>
-      </c>
-      <c r="C10" s="75">
-        <v>12</v>
-      </c>
-      <c r="D10" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="76" t="s">
-        <v>175</v>
-      </c>
-      <c r="G10" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="73">
-        <v>20220406</v>
-      </c>
-      <c r="I10" s="73">
-        <v>3</v>
-      </c>
-      <c r="J10" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="K10" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L10" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="73" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="73">
-        <v>7</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="76" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="73">
-        <v>20220406</v>
-      </c>
-      <c r="I11" s="73">
-        <v>3</v>
-      </c>
-      <c r="J11" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="K11" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="L11" s="73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" s="73">
-        <v>8</v>
-      </c>
-      <c r="C12" s="73">
-        <v>5</v>
-      </c>
-      <c r="D12" s="74" t="s">
-        <v>183</v>
-      </c>
-      <c r="E12" s="76" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="76" t="s">
-        <v>175</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>166</v>
-      </c>
-      <c r="H12" s="73">
-        <v>20220404</v>
-      </c>
-      <c r="I12" s="73">
-        <v>2</v>
-      </c>
-      <c r="J12" s="73" t="s">
-        <v>168</v>
-      </c>
-      <c r="K12" s="73" t="s">
-        <v>202</v>
-      </c>
-      <c r="L12" s="73" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="73" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4614,15 +5251,16 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68591B-911E-1D4D-A731-F1CC3E4BE9FA}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4630,117 +5268,146 @@
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
         <v>194</v>
-      </c>
-      <c r="B1" t="s">
-        <v>195</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="59">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="73">
-        <v>1</v>
-      </c>
-      <c r="B2" s="73" t="s">
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="59">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="73">
-        <v>2</v>
-      </c>
-      <c r="B3" s="73" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="59">
+        <v>3</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="73">
-        <v>3</v>
-      </c>
-      <c r="B4" s="73" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="59">
+        <v>4</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="73">
-        <v>4</v>
-      </c>
-      <c r="B5" s="73" t="s">
+      <c r="C5" s="59"/>
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="59">
+        <v>5</v>
+      </c>
+      <c r="B6" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="73">
-        <v>5</v>
-      </c>
-      <c r="B6" s="73" t="s">
+      <c r="C6" s="59"/>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="59">
+        <v>6</v>
+      </c>
+      <c r="B7" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="73">
-        <v>6</v>
-      </c>
-      <c r="B7" s="73" t="s">
+      <c r="C7" s="59"/>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="59">
+        <v>7</v>
+      </c>
+      <c r="B8" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="73">
-        <v>7</v>
-      </c>
-      <c r="B8" s="73" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="59">
+        <v>8</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="73">
-        <v>8</v>
-      </c>
-      <c r="B9" s="73" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="73"/>
+      <c r="C9" s="59"/>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>196</v>
+      </c>
+      <c r="E9" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trial6 V4 double check
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D5BA9A-85EA-E541-8725-E3FAA17240E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46B64B2-475C-CE48-A6BF-FC8E8C7673C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="460" windowWidth="28000" windowHeight="19560" activeTab="6" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="5600" yWindow="460" windowWidth="28000" windowHeight="19560" firstSheet="1" activeTab="7" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="Testing3 (338F) - 20220406" sheetId="5" r:id="rId5"/>
     <sheet name="Testing4 (341F) - 20220413" sheetId="9" r:id="rId6"/>
     <sheet name="Testing5 (Annealing Temp)" sheetId="10" r:id="rId7"/>
-    <sheet name="Sequencing URI GSC 1" sheetId="7" r:id="rId8"/>
-    <sheet name="Sequencing sheet for Janet 1" sheetId="8" r:id="rId9"/>
+    <sheet name="Testing6 (515F check)" sheetId="11" r:id="rId8"/>
+    <sheet name="Sequencing URI GSC 1" sheetId="7" r:id="rId9"/>
+    <sheet name="Sequencing sheet for Janet 1" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="276">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -809,9 +810,6 @@
     <t>Annealing Temperature</t>
   </si>
   <si>
-    <t>Testing higher annealing temperature using 338F - Trial #5</t>
-  </si>
-  <si>
     <t>60 C</t>
   </si>
   <si>
@@ -837,6 +835,42 @@
   </si>
   <si>
     <t>6. PCR start</t>
+  </si>
+  <si>
+    <t>Testing higher annealing temperature using 338F - Trial #5 - 20220418</t>
+  </si>
+  <si>
+    <t>Testing 515F primers on M. cap adults to see if DNA sample issue or V3 region issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 ng/uL DNA input for 2 temperatures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 ng/uL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20220406 8 ng/uL dilution strip tube </t>
+  </si>
+  <si>
+    <t>M-217 (Ext ID 16)</t>
+  </si>
+  <si>
+    <t>M-212 (Ext ID 17)</t>
+  </si>
+  <si>
+    <t>57 C</t>
+  </si>
+  <si>
+    <t>N (8*3*1.05)</t>
+  </si>
+  <si>
+    <t>515 F primer</t>
+  </si>
+  <si>
+    <t>806 RB primer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Grab reagents and DNA to thaw: Phusion, 515F and 806RB primers, 8 ng/uL stribe tube 20220406 </t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1368,6 +1402,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1922,6 +1957,163 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68591B-911E-1D4D-A731-F1CC3E4BE9FA}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="59">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="59">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="59">
+        <v>3</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="59">
+        <v>4</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="59">
+        <v>5</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="59">
+        <v>6</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="59">
+        <v>7</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="59">
+        <v>8</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="59"/>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A81F30F-E3B7-A04F-ABD2-645A1676EC1A}">
   <dimension ref="A1:C6"/>
@@ -4494,7 +4686,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4929,8 +5121,8 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4944,7 +5136,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="89" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="89"/>
@@ -4995,7 +5187,7 @@
         <v>252</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5012,7 +5204,7 @@
         <v>252</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5029,7 +5221,7 @@
         <v>252</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5046,7 +5238,7 @@
         <v>250</v>
       </c>
       <c r="E8" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5063,7 +5255,7 @@
         <v>252</v>
       </c>
       <c r="E9" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5080,7 +5272,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5097,7 +5289,7 @@
         <v>252</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5114,7 +5306,7 @@
         <v>252</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5131,7 +5323,7 @@
         <v>252</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -5148,7 +5340,7 @@
         <v>250</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -5165,7 +5357,7 @@
         <v>252</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5182,7 +5374,7 @@
         <v>43</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -5293,37 +5485,37 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -5338,6 +5530,338 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A49E82-F69A-7E4D-9CE1-1B85E69CD2D0}">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>3</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <v>4</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="91" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E9" s="67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E10" s="67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>7</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="25">
+        <v>8</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>12.5</v>
+      </c>
+      <c r="C18">
+        <f>8*3*1.05</f>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="D18" s="8">
+        <f>B18*C18</f>
+        <v>315.00000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C21" si="0">8*3*1.05</f>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" ref="D19:D21" si="1">B19*C19</f>
+        <v>12.600000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>274</v>
+      </c>
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="1"/>
+        <v>12.600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21">
+        <v>10.5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="D21" s="8">
+        <f t="shared" si="1"/>
+        <v>264.60000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f>SUM(D18:D21)</f>
+        <v>604.80000000000018</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f>D23/24</f>
+        <v>25.200000000000006</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="55" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E45E1A-AD6F-5D47-B9F5-6F99D46DA9AE}">
   <dimension ref="A1:N24"/>
   <sheetViews>
@@ -5737,161 +6261,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68591B-911E-1D4D-A731-F1CC3E4BE9FA}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="59">
-        <v>1</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="59"/>
-      <c r="D2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="59">
-        <v>2</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="59">
-        <v>3</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>185</v>
-      </c>
-      <c r="C4" s="59"/>
-      <c r="D4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="59">
-        <v>4</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" s="59"/>
-      <c r="D5" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="59">
-        <v>5</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="59">
-        <v>6</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="59"/>
-      <c r="D7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="59">
-        <v>7</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="C8" s="59"/>
-      <c r="D8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E8" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="59">
-        <v>8</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" s="59"/>
-      <c r="D9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cell counts AH post
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46B64B2-475C-CE48-A6BF-FC8E8C7673C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A076296D-691D-F74F-8E73-EBCDD9EF18FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5600" yWindow="460" windowWidth="28000" windowHeight="19560" firstSheet="1" activeTab="7" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
@@ -5531,10 +5531,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A49E82-F69A-7E4D-9CE1-1B85E69CD2D0}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5858,6 +5861,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
gel stitch and V3V4 updates
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A076296D-691D-F74F-8E73-EBCDD9EF18FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ACE915-60B9-BF42-A1E3-3C1182128C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="460" windowWidth="28000" windowHeight="19560" firstSheet="1" activeTab="7" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="1" activeTab="8" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="292">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -546,54 +546,18 @@
     <t>Band information</t>
   </si>
   <si>
-    <t>faint</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>strong</t>
-  </si>
-  <si>
     <t>DNA input</t>
   </si>
   <si>
     <t>8 ng/uL (24 ng total)</t>
   </si>
   <si>
-    <t>Pocillopora acuta</t>
-  </si>
-  <si>
-    <t>Porites asteroides</t>
-  </si>
-  <si>
-    <t>Montipora capitata</t>
-  </si>
-  <si>
-    <t>Lifestage</t>
-  </si>
-  <si>
-    <t>Settled recruit</t>
-  </si>
-  <si>
-    <t>Eggs</t>
-  </si>
-  <si>
-    <t>KW-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plug10 </t>
-  </si>
-  <si>
     <t>M-217</t>
   </si>
   <si>
     <t>M-212</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>ELS001</t>
   </si>
   <si>
@@ -621,9 +585,6 @@
     <t>Strip tube # to Janet</t>
   </si>
   <si>
-    <t>Original strip tube #</t>
-  </si>
-  <si>
     <t>Strip Tube #</t>
   </si>
   <si>
@@ -642,27 +603,12 @@
     <t xml:space="preserve">uL leftover after </t>
   </si>
   <si>
-    <t>3 (70 uL)</t>
-  </si>
-  <si>
     <t>Replicate # (uL total after gel)</t>
   </si>
   <si>
-    <t>2 (45 uL)</t>
-  </si>
-  <si>
-    <t>20 uL</t>
-  </si>
-  <si>
-    <t>45 uL</t>
-  </si>
-  <si>
     <t>4 ng/uL (12 ng total)</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>341F forward</t>
   </si>
   <si>
@@ -871,6 +817,108 @@
   </si>
   <si>
     <t xml:space="preserve">1. Grab reagents and DNA to thaw: Phusion, 515F and 806RB primers, 8 ng/uL stribe tube 20220406 </t>
+  </si>
+  <si>
+    <t>P. acuta 2513 adult</t>
+  </si>
+  <si>
+    <t>ELS009</t>
+  </si>
+  <si>
+    <t>ELS010</t>
+  </si>
+  <si>
+    <t>ELS011</t>
+  </si>
+  <si>
+    <t>ELS012</t>
+  </si>
+  <si>
+    <t>ELS013</t>
+  </si>
+  <si>
+    <t>ELS014</t>
+  </si>
+  <si>
+    <t>ELS015</t>
+  </si>
+  <si>
+    <t>20220406 Trial 3</t>
+  </si>
+  <si>
+    <t>Bright</t>
+  </si>
+  <si>
+    <t>16S Region</t>
+  </si>
+  <si>
+    <t>V3V4</t>
+  </si>
+  <si>
+    <t>Forward Primer Used</t>
+  </si>
+  <si>
+    <t>338F</t>
+  </si>
+  <si>
+    <t>P. ast KW-10 adult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bright </t>
+  </si>
+  <si>
+    <t>P. acuta 2878</t>
+  </si>
+  <si>
+    <t>20220321 Trial 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faint </t>
+  </si>
+  <si>
+    <t xml:space="preserve">63 C </t>
+  </si>
+  <si>
+    <t>20220418 Trial 5</t>
+  </si>
+  <si>
+    <t>341F</t>
+  </si>
+  <si>
+    <t>Plug 4 settled recruit</t>
+  </si>
+  <si>
+    <t>20220413 Trial 4</t>
+  </si>
+  <si>
+    <t>Very faint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">too low </t>
+  </si>
+  <si>
+    <t>ELS016</t>
+  </si>
+  <si>
+    <t>ELS017</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>515F</t>
+  </si>
+  <si>
+    <t>20220419 Trial 6</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>ELS018</t>
+  </si>
+  <si>
+    <t>ELS019</t>
   </si>
 </sst>
 </file>
@@ -1346,6 +1394,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1397,12 +1451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1733,12 +1781,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1759,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1798,16 +1846,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="E7" s="3">
         <v>50</v>
@@ -1821,10 +1869,10 @@
       <c r="C9" s="64"/>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="75"/>
+      <c r="B13" s="79"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1876,7 +1924,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1885,10 +1933,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="75" t="s">
-        <v>210</v>
-      </c>
-      <c r="B32" s="75"/>
+      <c r="A32" s="79" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" s="79"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
@@ -1897,7 +1945,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1938,7 +1986,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1972,19 +2020,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1992,14 +2040,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2007,14 +2055,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C3" s="59"/>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2022,14 +2070,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C4" s="59"/>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2037,14 +2085,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E5" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2052,14 +2100,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E6" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2067,14 +2115,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2082,14 +2130,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E8" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2097,14 +2145,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E9" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2156,7 +2204,7 @@
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="80" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2167,7 +2215,7 @@
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="80"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -2176,7 +2224,7 @@
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="76"/>
+      <c r="C5" s="80"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -2222,20 +2270,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -2266,16 +2314,16 @@
         <v>85</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -2692,12 +2740,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
       <c r="K16" s="5">
         <v>1</v>
       </c>
@@ -2846,12 +2894,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
       <c r="K24" s="5">
         <v>1</v>
       </c>
@@ -3055,32 +3103,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
@@ -3441,12 +3489,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -3496,12 +3544,12 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -3597,16 +3645,16 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="79"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
@@ -3801,17 +3849,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -4095,12 +4143,12 @@
       <c r="M13" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
@@ -4524,39 +4572,39 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85"/>
+      <c r="C33" s="88"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="88"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="89"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="86" t="s">
+      <c r="B34" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="88"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="91"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="92"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
       <c r="F37" s="55" t="s">
         <v>159</v>
       </c>
@@ -4702,33 +4750,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
-        <v>224</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="A1" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="88"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="B4" s="68" t="s">
         <v>140</v>
@@ -4737,19 +4785,19 @@
         <v>141</v>
       </c>
       <c r="D4" s="68" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -4763,7 +4811,7 @@
         <v>144</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>149</v>
@@ -4780,7 +4828,7 @@
         <v>144</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>151</v>
@@ -4797,7 +4845,7 @@
         <v>144</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>150</v>
@@ -4814,7 +4862,7 @@
         <v>144</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>150</v>
@@ -4831,7 +4879,7 @@
         <v>144</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>151</v>
@@ -4842,13 +4890,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="C10" s="67" t="s">
         <v>144</v>
       </c>
       <c r="D10" s="70" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="E10" s="69" t="s">
         <v>150</v>
@@ -4865,7 +4913,7 @@
         <v>16.862745098039216</v>
       </c>
       <c r="L10" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -4873,13 +4921,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="67" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>165</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>151</v>
@@ -4890,13 +4938,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="C12" s="67" t="s">
         <v>165</v>
       </c>
       <c r="D12" s="69" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>151</v>
@@ -4913,7 +4961,7 @@
         <v>144</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>149</v>
@@ -4947,47 +4995,47 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="B21" s="67"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
       <c r="F27" s="55" t="s">
         <v>159</v>
       </c>
@@ -4997,7 +5045,7 @@
         <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>54</v>
@@ -5041,10 +5089,10 @@
         <v>15.75</v>
       </c>
       <c r="F30" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="G30" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -5063,7 +5111,7 @@
         <v>15.75</v>
       </c>
       <c r="G31" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -5082,7 +5130,7 @@
         <v>330.75</v>
       </c>
       <c r="G32" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.2">
@@ -5135,30 +5183,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="A1" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="90" t="s">
-        <v>248</v>
-      </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="A2" s="94" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>140</v>
@@ -5167,10 +5215,10 @@
         <v>141</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5178,16 +5226,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5198,13 +5246,13 @@
         <v>143</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5212,16 +5260,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="C7" s="67" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5229,16 +5277,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="67" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="E8" s="67" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5246,33 +5294,33 @@
         <v>5</v>
       </c>
       <c r="B9" s="67" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E9" s="67" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>6</v>
       </c>
-      <c r="B10" s="91" t="s">
-        <v>253</v>
-      </c>
-      <c r="C10" s="91" t="s">
+      <c r="B10" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="91" t="s">
-        <v>255</v>
+      <c r="E10" s="74" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5280,16 +5328,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5300,13 +5348,13 @@
         <v>143</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5314,16 +5362,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="67" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -5331,16 +5379,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="67" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -5348,16 +5396,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="67" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5365,7 +5413,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="67" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="C16" s="67" t="s">
         <v>43</v>
@@ -5374,11 +5422,11 @@
         <v>43</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="76" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="73"/>
@@ -5480,42 +5528,42 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="55" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -5536,7 +5584,7 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -5550,26 +5598,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
-        <v>265</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="A1" s="93" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>140</v>
@@ -5578,10 +5626,10 @@
         <v>141</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5589,16 +5637,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5606,16 +5654,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5626,30 +5674,30 @@
         <v>143</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>4</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="74" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>267</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="91" t="s">
-        <v>271</v>
+        <v>249</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5657,16 +5705,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E9" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5674,16 +5722,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5694,13 +5742,13 @@
         <v>143</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5711,17 +5759,17 @@
         <v>40</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="76" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="73"/>
@@ -5733,7 +5781,7 @@
         <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>54</v>
@@ -5757,7 +5805,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="B19">
         <v>0.5</v>
@@ -5773,7 +5821,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="B20">
         <v>0.5</v>
@@ -5823,37 +5871,37 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="55" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -5867,399 +5915,783 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E45E1A-AD6F-5D47-B9F5-6F99D46DA9AE}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" style="59" customWidth="1"/>
     <col min="2" max="2" width="20" style="59" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="59" customWidth="1"/>
-    <col min="4" max="6" width="19.83203125" style="59" customWidth="1"/>
-    <col min="7" max="7" width="22" style="59" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="59" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="59"/>
-    <col min="10" max="10" width="16.83203125" style="59" customWidth="1"/>
-    <col min="11" max="11" width="26.1640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15" style="59" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="59" customWidth="1"/>
+    <col min="5" max="5" width="22" style="59" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="59" customWidth="1"/>
+    <col min="7" max="8" width="19.83203125" style="59" customWidth="1"/>
+    <col min="9" max="10" width="26.1640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="59" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="59" customWidth="1"/>
+    <col min="13" max="13" width="26.1640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="93" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-    </row>
-    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+    </row>
+    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="58" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="E4" s="58" t="s">
-        <v>175</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" s="58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H4" s="58" t="s">
         <v>164</v>
       </c>
       <c r="I4" s="58" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="J4" s="58" t="s">
-        <v>166</v>
-      </c>
-      <c r="K4" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B5" s="59">
         <v>1</v>
       </c>
-      <c r="C5" s="61">
-        <v>7</v>
-      </c>
-      <c r="D5" s="59">
-        <v>2513</v>
+      <c r="C5" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>271</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>258</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J5" s="59">
+        <v>3</v>
+      </c>
+      <c r="K5" s="59">
+        <f>70-25</f>
+        <v>45</v>
+      </c>
+      <c r="N5" s="59"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="59" t="s">
         <v>172</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="H5" s="59">
-        <v>20220406</v>
-      </c>
-      <c r="I5" s="59">
-        <v>3</v>
-      </c>
-      <c r="J5" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="K5" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L5" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
-        <v>184</v>
       </c>
       <c r="B6" s="59">
         <v>2</v>
       </c>
-      <c r="C6" s="61">
-        <v>8</v>
+      <c r="C6" s="59" t="s">
+        <v>269</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>178</v>
+        <v>271</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="F6" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J6" s="59">
+        <v>3</v>
+      </c>
+      <c r="K6" s="59">
+        <f>70-25</f>
+        <v>45</v>
+      </c>
+      <c r="N6" s="59"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="59" t="s">
         <v>173</v>
-      </c>
-      <c r="G6" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="H6" s="59">
-        <v>20220406</v>
-      </c>
-      <c r="I6" s="59">
-        <v>3</v>
-      </c>
-      <c r="J6" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="K6" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L6" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
-        <v>185</v>
       </c>
       <c r="B7" s="59">
         <v>3</v>
       </c>
-      <c r="C7" s="61">
-        <v>9</v>
-      </c>
-      <c r="D7" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>176</v>
+      <c r="C7" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>253</v>
       </c>
       <c r="F7" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>273</v>
+      </c>
+      <c r="J7" s="59">
+        <v>3</v>
+      </c>
+      <c r="K7" s="59">
+        <f>70-25</f>
+        <v>45</v>
+      </c>
+      <c r="N7" s="59"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="59" t="s">
         <v>174</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="H7" s="59">
-        <v>20220406</v>
-      </c>
-      <c r="I7" s="59">
-        <v>3</v>
-      </c>
-      <c r="J7" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="K7" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L7" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
-        <v>186</v>
       </c>
       <c r="B8" s="59">
         <v>4</v>
       </c>
-      <c r="C8" s="61">
-        <v>10</v>
-      </c>
-      <c r="D8" s="59">
-        <v>2878</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="G8" s="59" t="s">
-        <v>204</v>
-      </c>
-      <c r="H8" s="59">
-        <v>20220321</v>
-      </c>
-      <c r="I8" s="59">
-        <v>1</v>
-      </c>
-      <c r="J8" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="K8" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L8" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>275</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>276</v>
+      </c>
+      <c r="J8" s="59">
+        <v>2</v>
+      </c>
+      <c r="K8" s="59">
+        <f>45-25</f>
+        <v>20</v>
+      </c>
+      <c r="N8" s="59"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B9" s="59">
         <v>5</v>
       </c>
-      <c r="C9" s="61">
-        <v>11</v>
+      <c r="C9" s="59" t="s">
+        <v>269</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>174</v>
-      </c>
-      <c r="G9" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="H9" s="59">
-        <v>20220406</v>
-      </c>
-      <c r="I9" s="59">
-        <v>3</v>
-      </c>
-      <c r="J9" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="K9" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L9" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>283</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>275</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>276</v>
+      </c>
+      <c r="J9" s="59">
+        <v>2</v>
+      </c>
+      <c r="K9" s="59">
+        <f>45-25</f>
+        <v>20</v>
+      </c>
+      <c r="N9" s="59"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B10" s="59">
         <v>6</v>
       </c>
-      <c r="C10" s="61">
-        <v>12</v>
-      </c>
-      <c r="D10" s="60" t="s">
-        <v>181</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>174</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" s="59">
-        <v>20220406</v>
-      </c>
-      <c r="I10" s="59">
+      <c r="C10" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>278</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J10" s="59">
         <v>3</v>
       </c>
-      <c r="J10" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="K10" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L10" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K10" s="59">
+        <f t="shared" ref="K10:K23" si="0">70-25</f>
+        <v>45</v>
+      </c>
+      <c r="N10" s="59"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="59" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B11" s="59">
         <v>7</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="D11" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="59" t="s">
-        <v>43</v>
+        <v>271</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>277</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>43</v>
+        <v>272</v>
       </c>
       <c r="G11" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="59">
-        <v>20220406</v>
-      </c>
-      <c r="I11" s="59">
+        <v>187</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>278</v>
+      </c>
+      <c r="I11" s="62" t="s">
+        <v>267</v>
+      </c>
+      <c r="J11" s="59">
         <v>3</v>
       </c>
-      <c r="J11" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="K11" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="L11" s="59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K11" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="N11" s="59"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B12" s="59">
         <v>8</v>
       </c>
-      <c r="C12" s="59">
-        <v>5</v>
-      </c>
-      <c r="D12" s="60" t="s">
-        <v>182</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="62" t="s">
-        <v>174</v>
+      <c r="C12" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>231</v>
       </c>
       <c r="G12" s="62" t="s">
-        <v>165</v>
-      </c>
-      <c r="H12" s="59">
-        <v>20220404</v>
-      </c>
-      <c r="I12" s="59">
-        <v>2</v>
-      </c>
-      <c r="J12" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="K12" s="59" t="s">
-        <v>201</v>
-      </c>
-      <c r="L12" s="59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="59" t="s">
-        <v>205</v>
+        <v>187</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>278</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>276</v>
+      </c>
+      <c r="J12" s="59">
+        <v>3</v>
+      </c>
+      <c r="K12" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="N12" s="59"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" s="59">
+        <v>9</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>258</v>
+      </c>
+      <c r="G13" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="I13" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J13" s="59">
+        <v>3</v>
+      </c>
+      <c r="K13" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="59" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" s="59">
+        <v>10</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H14" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="I14" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J14" s="59">
+        <v>3</v>
+      </c>
+      <c r="K14" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="59" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="59">
+        <v>11</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>276</v>
+      </c>
+      <c r="J15" s="59">
+        <v>3</v>
+      </c>
+      <c r="K15" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="59" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" s="59">
+        <v>12</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>280</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>276</v>
+      </c>
+      <c r="J16" s="59">
+        <v>3</v>
+      </c>
+      <c r="K16" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="59" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" s="59">
+        <v>13</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>283</v>
+      </c>
+      <c r="H17" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="I17" s="59" t="s">
+        <v>282</v>
+      </c>
+      <c r="J17" s="59">
+        <v>3</v>
+      </c>
+      <c r="K17" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="59" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="59">
+        <v>14</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="I18" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J18" s="59">
+        <v>3</v>
+      </c>
+      <c r="K18" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="59" t="s">
+        <v>265</v>
+      </c>
+      <c r="B19" s="59">
+        <v>15</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="I19" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J19" s="59">
+        <v>3</v>
+      </c>
+      <c r="K19" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" s="59">
+        <v>16</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H20" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="I20" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J20" s="59">
+        <v>3</v>
+      </c>
+      <c r="K20" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="59" t="s">
+        <v>285</v>
+      </c>
+      <c r="B21" s="59">
+        <v>17</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="I21" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="J21" s="59">
+        <v>3</v>
+      </c>
+      <c r="K21" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="59" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" s="59">
+        <v>18</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="E22" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="F22" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="I22" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="J22" s="59">
+        <v>3</v>
+      </c>
+      <c r="K22" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="59" t="s">
+        <v>291</v>
+      </c>
+      <c r="B23" s="59">
+        <v>19</v>
+      </c>
+      <c r="C23" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="I23" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="J23" s="59">
+        <v>3</v>
+      </c>
+      <c r="K23" s="59">
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
NGS submission sheet and scanned image
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2A48E2-EEEC-FA43-9095-E0ABBB2D090F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA31D9F7-80AB-3C4F-9636-A9901BF2BF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="1" activeTab="8" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="5660" yWindow="460" windowWidth="27940" windowHeight="19560" firstSheet="4" activeTab="9" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="348">
   <si>
     <t>Putnam Lab V3V4 16S sequencing</t>
   </si>
@@ -558,6 +558,9 @@
     <t>M-212</t>
   </si>
   <si>
+    <t>D1</t>
+  </si>
+  <si>
     <t>ELS001</t>
   </si>
   <si>
@@ -582,9 +585,6 @@
     <t>ELS008</t>
   </si>
   <si>
-    <t>Strip Tube #</t>
-  </si>
-  <si>
     <t>Sample ID</t>
   </si>
   <si>
@@ -925,13 +925,175 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>ELS020</t>
+  </si>
+  <si>
+    <t>ELS021</t>
+  </si>
+  <si>
+    <t>ELS022</t>
+  </si>
+  <si>
+    <t>ELS023</t>
+  </si>
+  <si>
+    <t>ELS024</t>
+  </si>
+  <si>
+    <t>ELS025</t>
+  </si>
+  <si>
+    <t>ELS026</t>
+  </si>
+  <si>
+    <t>ELS027</t>
+  </si>
+  <si>
+    <t>ELS028</t>
+  </si>
+  <si>
+    <t>ELS029</t>
+  </si>
+  <si>
+    <t>ELS030</t>
+  </si>
+  <si>
+    <t>ITS2</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>ITSintfor2</t>
+  </si>
+  <si>
+    <t>52 C</t>
+  </si>
+  <si>
+    <t>R36-A2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>R28-A2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>R7-A4</t>
+  </si>
+  <si>
+    <t>R35-A4</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>R36-A4</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>R19-A4</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>R26-A2</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>R28-A4</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>R37-A4</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>R29-A4</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>R8-A4</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>Well ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1062,6 +1224,31 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1303,7 +1490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1370,19 +1557,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1456,6 +1631,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,12 +1989,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1857,7 +2059,7 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="61" t="s">
         <v>188</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1868,17 +2070,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="C8" s="65"/>
-      <c r="D8" s="66"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="C9" s="64"/>
+      <c r="C9" s="60"/>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="79"/>
+      <c r="B13" s="75"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1939,10 +2141,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="B32" s="79"/>
+      <c r="B32" s="75"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
@@ -2013,10 +2215,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68591B-911E-1D4D-A731-F1CC3E4BE9FA}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2025,139 +2227,529 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="95" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="95" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="95" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="95" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="95" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="95" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="95" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="95" t="s">
+        <v>321</v>
+      </c>
+      <c r="B9" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="59">
-        <v>1</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="59"/>
-      <c r="D2" t="s">
+      <c r="C9" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="95" t="s">
+        <v>323</v>
+      </c>
+      <c r="B10" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="95" t="s">
+        <v>325</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="95" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" s="102" t="s">
+        <v>305</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="95" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="C13" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E13" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="59">
-        <v>2</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="95" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E14" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="59">
-        <v>3</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="59"/>
-      <c r="D4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="95" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D15" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E15" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="59">
-        <v>4</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="59"/>
-      <c r="D5" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="95" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D16" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E16" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="59">
-        <v>5</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="95" t="s">
+        <v>333</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="C17" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E17" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="59">
-        <v>6</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="59"/>
-      <c r="D7" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="95" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>282</v>
+      </c>
+      <c r="C18" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D18" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E18" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="59">
-        <v>7</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="59"/>
-      <c r="D8" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D19" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E19" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="59">
-        <v>8</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="59"/>
-      <c r="D9" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="95" t="s">
+        <v>335</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E20" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="C21" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="B22" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D22" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="B23" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="C23" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D23" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="95" t="s">
+        <v>339</v>
+      </c>
+      <c r="B24" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="95" t="s">
+        <v>340</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D25" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="95" t="s">
+        <v>341</v>
+      </c>
+      <c r="B26" s="91" t="s">
+        <v>299</v>
+      </c>
+      <c r="C26" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="D26" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="95" t="s">
+        <v>342</v>
+      </c>
+      <c r="B27" s="91" t="s">
+        <v>300</v>
+      </c>
+      <c r="C27" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="D27" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="95" t="s">
+        <v>343</v>
+      </c>
+      <c r="B28" s="91" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="D28" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="95" t="s">
+        <v>344</v>
+      </c>
+      <c r="B29" s="91" t="s">
+        <v>302</v>
+      </c>
+      <c r="C29" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D29" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="95" t="s">
+        <v>345</v>
+      </c>
+      <c r="B30" s="91" t="s">
+        <v>303</v>
+      </c>
+      <c r="C30" s="91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D30" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="95" t="s">
+        <v>346</v>
+      </c>
+      <c r="B31" s="91" t="s">
+        <v>304</v>
+      </c>
+      <c r="C31" s="91" t="s">
+        <v>283</v>
+      </c>
+      <c r="D31" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2210,7 +2802,7 @@
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="76" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2221,7 +2813,7 @@
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="80"/>
+      <c r="C4" s="76"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -2230,7 +2822,7 @@
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="80"/>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -2276,20 +2868,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -2320,16 +2912,16 @@
         <v>85</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="83" t="s">
+      <c r="K3" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -2746,12 +3338,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
       <c r="K16" s="5">
         <v>1</v>
       </c>
@@ -2900,12 +3492,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
       <c r="K24" s="5">
         <v>1</v>
       </c>
@@ -3109,32 +3701,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
@@ -3495,12 +4087,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -3550,12 +4142,12 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -3651,16 +4243,16 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="s">
+      <c r="A35" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
@@ -3855,17 +4447,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -4149,12 +4741,12 @@
       <c r="M13" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
@@ -4578,39 +5170,39 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="88"/>
-      <c r="H33" s="88"/>
-      <c r="I33" s="89"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="90" t="s">
+      <c r="B34" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="92"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="88"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
       <c r="F37" s="55" t="s">
         <v>159</v>
       </c>
@@ -4756,41 +5348,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="88"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="64" t="s">
         <v>197</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -4898,23 +5490,23 @@
       <c r="B10" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="66" t="s">
         <v>211</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="65" t="s">
         <v>150</v>
       </c>
       <c r="F10" s="6">
         <v>51</v>
       </c>
-      <c r="G10" s="71">
+      <c r="G10" s="67">
         <f>160/F10</f>
         <v>3.1372549019607843</v>
       </c>
-      <c r="H10" s="72">
+      <c r="H10" s="68">
         <f>20-G10</f>
         <v>16.862745098039216</v>
       </c>
@@ -4926,13 +5518,13 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="65" t="s">
         <v>199</v>
       </c>
       <c r="E11" s="33" t="s">
@@ -4943,13 +5535,13 @@
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="65" t="s">
         <v>213</v>
       </c>
       <c r="E12" s="33" t="s">
@@ -4977,25 +5569,25 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="67" t="s">
+      <c r="G14" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="67" t="s">
+      <c r="H14" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5023,7 +5615,7 @@
       <c r="A21" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="63"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -5036,12 +5628,12 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
       <c r="F27" s="55" t="s">
         <v>159</v>
       </c>
@@ -5189,26 +5781,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="89" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="90" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -5240,7 +5832,7 @@
       <c r="D5" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="63" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5257,7 +5849,7 @@
       <c r="D6" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="63" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5265,16 +5857,16 @@
       <c r="A7" s="25">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="63" t="s">
         <v>228</v>
       </c>
       <c r="D7" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="63" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5282,16 +5874,16 @@
       <c r="A8" s="25">
         <v>4</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="63" t="s">
         <v>232</v>
       </c>
       <c r="D8" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="63" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5299,16 +5891,16 @@
       <c r="A9" s="25">
         <v>5</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="63" t="s">
         <v>228</v>
       </c>
       <c r="D9" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="63" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5316,16 +5908,16 @@
       <c r="A10" s="28">
         <v>6</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="70" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5342,7 +5934,7 @@
       <c r="D11" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5359,7 +5951,7 @@
       <c r="D12" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5367,16 +5959,16 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="63" t="s">
         <v>228</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5384,16 +5976,16 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="63" t="s">
         <v>232</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5401,16 +5993,16 @@
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="63" t="s">
         <v>228</v>
       </c>
       <c r="D15" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5418,26 +6010,26 @@
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="63" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="63" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -5604,17 +6196,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="89" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -5651,7 +6243,7 @@
       <c r="D5" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="63" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5668,7 +6260,7 @@
       <c r="D6" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="63" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5685,7 +6277,7 @@
       <c r="D7" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="63" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5693,16 +6285,16 @@
       <c r="A8" s="28">
         <v>4</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="70" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="73" t="s">
         <v>231</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="70" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5719,7 +6311,7 @@
       <c r="D9" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5736,7 +6328,7 @@
       <c r="D10" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="E10" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5753,7 +6345,7 @@
       <c r="D11" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="63" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5761,7 +6353,7 @@
       <c r="A12" s="25">
         <v>8</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="25" t="s">
@@ -5770,17 +6362,17 @@
       <c r="D12" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="63" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
@@ -5921,790 +6513,1473 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E45E1A-AD6F-5D47-B9F5-6F99D46DA9AE}">
-  <dimension ref="A1:Q23"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="59" customWidth="1"/>
-    <col min="2" max="3" width="20" style="59" customWidth="1"/>
-    <col min="4" max="4" width="15" style="59" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="59" customWidth="1"/>
-    <col min="6" max="6" width="22" style="59" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="59" customWidth="1"/>
-    <col min="8" max="9" width="19.83203125" style="59" customWidth="1"/>
-    <col min="10" max="11" width="26.1640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="59" customWidth="1"/>
-    <col min="14" max="14" width="26.1640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="58" customWidth="1"/>
+    <col min="2" max="2" width="20" style="58" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="15" style="58" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="58" customWidth="1"/>
+    <col min="6" max="6" width="14" style="58" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="58" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="58" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="58" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" style="58" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="58" customWidth="1"/>
+    <col min="12" max="12" width="11" style="58" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="58" customWidth="1"/>
+    <col min="14" max="14" width="26.1640625" style="58" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="59" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+    <row r="4" spans="1:17" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="94" t="s">
         <v>291</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="100" t="s">
         <v>292</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="101" t="s">
         <v>268</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="94" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="94" t="s">
         <v>164</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="94" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="101" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="95" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F5" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G5" s="95">
+        <v>12</v>
+      </c>
+      <c r="H5" s="95" t="s">
+        <v>309</v>
+      </c>
+      <c r="I5" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="93"/>
+      <c r="O5" s="58"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F6" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G6" s="95">
+        <v>72</v>
+      </c>
+      <c r="H6" s="95" t="s">
+        <v>311</v>
+      </c>
+      <c r="I6" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="93"/>
+      <c r="O6" s="58"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F7" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G7" s="95">
+        <v>78</v>
+      </c>
+      <c r="H7" s="95" t="s">
+        <v>313</v>
+      </c>
+      <c r="I7" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="93"/>
+      <c r="O7" s="58"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C8" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F8" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G8" s="95">
+        <v>84</v>
+      </c>
+      <c r="H8" s="95" t="s">
+        <v>314</v>
+      </c>
+      <c r="I8" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="93"/>
+      <c r="O8" s="58"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E9" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F9" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G9" s="95">
+        <v>120</v>
+      </c>
+      <c r="H9" s="95" t="s">
+        <v>316</v>
+      </c>
+      <c r="I9" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="93"/>
+      <c r="O9" s="58"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="95" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="95" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F10" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G10" s="95">
+        <v>132</v>
+      </c>
+      <c r="H10" s="95" t="s">
+        <v>318</v>
+      </c>
+      <c r="I10" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="93"/>
+      <c r="O10" s="58"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="95" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>319</v>
+      </c>
+      <c r="C11" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E11" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G11" s="95">
+        <v>138</v>
+      </c>
+      <c r="H11" s="95" t="s">
+        <v>320</v>
+      </c>
+      <c r="I11" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="93"/>
+      <c r="O11" s="58"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E12" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F12" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G12" s="95">
+        <v>144</v>
+      </c>
+      <c r="H12" s="95" t="s">
+        <v>322</v>
+      </c>
+      <c r="I12" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K12" s="97"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="93"/>
+      <c r="O12" s="58"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D13" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F13" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G13" s="95">
+        <v>168</v>
+      </c>
+      <c r="H13" s="95" t="s">
+        <v>324</v>
+      </c>
+      <c r="I13" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="93"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="95" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D14" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F14" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G14" s="95">
+        <v>204</v>
+      </c>
+      <c r="H14" s="95" t="s">
+        <v>326</v>
+      </c>
+      <c r="I14" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="93"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="95" t="s">
+        <v>260</v>
+      </c>
+      <c r="B15" s="95" t="s">
+        <v>327</v>
+      </c>
+      <c r="C15" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" s="95" t="s">
+        <v>305</v>
+      </c>
+      <c r="E15" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="F15" s="95" t="s">
+        <v>308</v>
+      </c>
+      <c r="G15" s="95">
+        <v>210</v>
+      </c>
+      <c r="H15" s="95" t="s">
+        <v>328</v>
+      </c>
+      <c r="I15" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="95">
+        <v>20220321</v>
+      </c>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="93"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="95" t="s">
+        <v>329</v>
+      </c>
+      <c r="C16" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D16" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E16" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F16" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G16" s="98" t="s">
         <v>257</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H16" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I16" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J16" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K5" s="59">
+      <c r="K16" s="91">
         <v>3</v>
       </c>
-      <c r="L5" s="59">
+      <c r="L16" s="91">
         <f>70-25</f>
         <v>45</v>
       </c>
-      <c r="O5" s="59"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="59" t="s">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="B17" s="95" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D17" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E17" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F17" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G17" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H17" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I17" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J17" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K6" s="59">
+      <c r="K17" s="91">
         <v>3</v>
       </c>
-      <c r="L6" s="59">
+      <c r="L17" s="91">
         <f>70-25</f>
         <v>45</v>
       </c>
-      <c r="O6" s="59"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="59" t="s">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" s="95" t="s">
+        <v>331</v>
+      </c>
+      <c r="C18" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D18" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E18" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F18" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G18" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H18" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I18" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J18" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="K7" s="59">
+      <c r="K18" s="91">
         <v>3</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L18" s="91">
         <f>70-25</f>
         <v>45</v>
       </c>
-      <c r="O7" s="59"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="59" t="s">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="95" t="s">
+        <v>332</v>
+      </c>
+      <c r="C19" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D19" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E19" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F19" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G19" s="91" t="s">
         <v>272</v>
       </c>
-      <c r="H8" s="62" t="s">
+      <c r="H19" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="I8" s="62" t="s">
+      <c r="I19" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J19" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="K8" s="59">
+      <c r="K19" s="91">
         <v>2</v>
       </c>
-      <c r="L8" s="59">
+      <c r="L19" s="91">
         <f>45-25</f>
         <v>20</v>
       </c>
-      <c r="O8" s="59"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="59" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="59" t="s">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="B20" s="95" t="s">
+        <v>333</v>
+      </c>
+      <c r="C20" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D20" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E20" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F20" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G20" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="H9" s="62" t="s">
+      <c r="H20" s="99" t="s">
         <v>280</v>
       </c>
-      <c r="I9" s="62" t="s">
+      <c r="I20" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J20" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K20" s="91">
         <v>2</v>
       </c>
-      <c r="L9" s="59">
+      <c r="L20" s="91">
         <f>45-25</f>
         <v>20</v>
       </c>
-      <c r="O9" s="59"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="59" t="s">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="91" t="s">
+        <v>282</v>
+      </c>
+      <c r="B21" s="95" t="s">
+        <v>334</v>
+      </c>
+      <c r="C21" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D21" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E21" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F21" s="98" t="s">
         <v>274</v>
       </c>
-      <c r="G10" s="61" t="s">
+      <c r="G21" s="98" t="s">
         <v>257</v>
       </c>
-      <c r="H10" s="62" t="s">
+      <c r="H21" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="I10" s="62" t="s">
+      <c r="I21" s="99" t="s">
         <v>275</v>
       </c>
-      <c r="J10" s="59" t="s">
+      <c r="J21" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K10" s="59">
+      <c r="K21" s="91">
         <v>3</v>
       </c>
-      <c r="L10" s="59">
-        <f t="shared" ref="L10:L23" si="0">70-25</f>
+      <c r="L21" s="91">
+        <f t="shared" ref="L21:L34" si="0">70-25</f>
         <v>45</v>
       </c>
-      <c r="O10" s="59"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="C11" s="59" t="s">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="B22" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D22" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E22" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F11" s="61" t="s">
+      <c r="F22" s="98" t="s">
         <v>274</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G22" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="H22" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="I11" s="62" t="s">
+      <c r="I22" s="99" t="s">
         <v>275</v>
       </c>
-      <c r="J11" s="62" t="s">
+      <c r="J22" s="99" t="s">
         <v>266</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K22" s="91">
         <v>3</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L22" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="O11" s="59"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="59" t="s">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23" s="95" t="s">
+        <v>335</v>
+      </c>
+      <c r="C23" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D23" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E23" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F12" s="61" t="s">
+      <c r="F23" s="98" t="s">
         <v>274</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G23" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="H12" s="62" t="s">
+      <c r="H23" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="I12" s="62" t="s">
+      <c r="I23" s="99" t="s">
         <v>275</v>
       </c>
-      <c r="J12" s="62" t="s">
+      <c r="J23" s="99" t="s">
         <v>273</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K23" s="91">
         <v>3</v>
       </c>
-      <c r="L12" s="59">
+      <c r="L23" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="O12" s="59"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" s="59" t="s">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="C24" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D24" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E24" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F24" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G24" s="91" t="s">
         <v>257</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H24" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I24" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="J13" s="59" t="s">
+      <c r="J24" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K24" s="91">
         <v>3</v>
       </c>
-      <c r="L13" s="59">
+      <c r="L24" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="59" t="s">
-        <v>259</v>
-      </c>
-      <c r="C14" s="59" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="B25" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="C25" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D25" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E25" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F25" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G25" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="H14" s="59" t="s">
+      <c r="H25" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I25" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J25" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K14" s="59">
+      <c r="K25" s="91">
         <v>3</v>
       </c>
-      <c r="L14" s="59">
+      <c r="L25" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
-        <v>260</v>
-      </c>
-      <c r="C15" s="59" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="B26" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="C26" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D26" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E26" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F26" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G15" s="59" t="s">
+      <c r="G26" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H26" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I26" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="J15" s="59" t="s">
+      <c r="J26" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K26" s="91">
         <v>3</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L26" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>261</v>
-      </c>
-      <c r="C16" s="59" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="95" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D27" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E27" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="F16" s="59" t="s">
+      <c r="F27" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G16" s="59" t="s">
+      <c r="G27" s="91" t="s">
         <v>277</v>
       </c>
-      <c r="H16" s="59" t="s">
+      <c r="H27" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="I27" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="J16" s="59" t="s">
+      <c r="J27" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="K16" s="59">
+      <c r="K27" s="91">
         <v>3</v>
       </c>
-      <c r="L16" s="59">
+      <c r="L27" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
-        <v>262</v>
-      </c>
-      <c r="C17" s="59" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="91" t="s">
+        <v>298</v>
+      </c>
+      <c r="B28" s="95" t="s">
+        <v>340</v>
+      </c>
+      <c r="C28" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D28" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E28" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F28" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G28" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="H28" s="99" t="s">
         <v>280</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I28" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="J17" s="59" t="s">
+      <c r="J28" s="91" t="s">
         <v>279</v>
       </c>
-      <c r="K17" s="59">
+      <c r="K28" s="91">
         <v>3</v>
       </c>
-      <c r="L17" s="59">
+      <c r="L28" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="s">
-        <v>263</v>
-      </c>
-      <c r="C18" s="59" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="91" t="s">
+        <v>299</v>
+      </c>
+      <c r="B29" s="95" t="s">
+        <v>341</v>
+      </c>
+      <c r="C29" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D29" s="91" t="s">
         <v>283</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E29" s="91" t="s">
         <v>284</v>
       </c>
-      <c r="F18" s="59" t="s">
+      <c r="F29" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G29" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="59" t="s">
+      <c r="H29" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="I29" s="91" t="s">
         <v>285</v>
       </c>
-      <c r="J18" s="59" t="s">
+      <c r="J29" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K18" s="59">
+      <c r="K29" s="91">
         <v>3</v>
       </c>
-      <c r="L18" s="59">
+      <c r="L29" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="59" t="s">
-        <v>264</v>
-      </c>
-      <c r="C19" s="59" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="91" t="s">
+        <v>300</v>
+      </c>
+      <c r="B30" s="95" t="s">
+        <v>342</v>
+      </c>
+      <c r="C30" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D30" s="91" t="s">
         <v>283</v>
       </c>
-      <c r="E19" s="59" t="s">
+      <c r="E30" s="91" t="s">
         <v>284</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F30" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="G19" s="59" t="s">
+      <c r="G30" s="91" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="59" t="s">
+      <c r="H30" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I30" s="91" t="s">
         <v>285</v>
       </c>
-      <c r="J19" s="59" t="s">
+      <c r="J30" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K19" s="59">
+      <c r="K30" s="91">
         <v>3</v>
       </c>
-      <c r="L19" s="59">
+      <c r="L30" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" s="59" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="91" t="s">
+        <v>301</v>
+      </c>
+      <c r="B31" s="95" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D31" s="91" t="s">
         <v>283</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E31" s="91" t="s">
         <v>284</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F31" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="G20" s="59" t="s">
+      <c r="G31" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="H20" s="59" t="s">
+      <c r="H31" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="I20" s="59" t="s">
+      <c r="I31" s="91" t="s">
         <v>285</v>
       </c>
-      <c r="J20" s="59" t="s">
+      <c r="J31" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="K20" s="59">
+      <c r="K31" s="91">
         <v>3</v>
       </c>
-      <c r="L20" s="59">
+      <c r="L31" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="59" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" s="59" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="91" t="s">
+        <v>302</v>
+      </c>
+      <c r="B32" s="95" t="s">
+        <v>344</v>
+      </c>
+      <c r="C32" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D32" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E32" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="F32" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G21" s="61" t="s">
+      <c r="G32" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H32" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="I32" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="J21" s="59" t="s">
+      <c r="J32" s="91" t="s">
         <v>286</v>
       </c>
-      <c r="K21" s="59">
+      <c r="K32" s="91">
         <v>3</v>
       </c>
-      <c r="L21" s="59">
+      <c r="L32" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="59" t="s">
-        <v>287</v>
-      </c>
-      <c r="C22" s="59" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="91" t="s">
+        <v>303</v>
+      </c>
+      <c r="B33" s="95" t="s">
+        <v>345</v>
+      </c>
+      <c r="C33" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D33" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E33" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="F22" s="59" t="s">
+      <c r="F33" s="91" t="s">
         <v>252</v>
       </c>
-      <c r="G22" s="61" t="s">
+      <c r="G33" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H33" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="I33" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="J33" s="91" t="s">
         <v>286</v>
       </c>
-      <c r="K22" s="59">
+      <c r="K33" s="91">
         <v>3</v>
       </c>
-      <c r="L22" s="59">
+      <c r="L33" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="59" t="s">
-        <v>288</v>
-      </c>
-      <c r="C23" s="59" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="91" t="s">
+        <v>304</v>
+      </c>
+      <c r="B34" s="95" t="s">
+        <v>346</v>
+      </c>
+      <c r="C34" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="59" t="s">
+      <c r="D34" s="91" t="s">
         <v>283</v>
       </c>
-      <c r="E23" s="59" t="s">
+      <c r="E34" s="91" t="s">
         <v>284</v>
       </c>
-      <c r="F23" s="59" t="s">
+      <c r="F34" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="G23" s="61" t="s">
+      <c r="G34" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H34" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="59" t="s">
+      <c r="I34" s="91" t="s">
         <v>285</v>
       </c>
-      <c r="J23" s="59" t="s">
+      <c r="J34" s="91" t="s">
         <v>286</v>
       </c>
-      <c r="K23" s="59">
+      <c r="K34" s="91">
         <v>3</v>
       </c>
-      <c r="L23" s="59">
+      <c r="L34" s="91">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="91"/>
+      <c r="B38" s="91">
+        <v>1</v>
+      </c>
+      <c r="C38" s="91">
+        <v>2</v>
+      </c>
+      <c r="D38" s="91">
+        <v>3</v>
+      </c>
+      <c r="E38" s="91">
+        <v>4</v>
+      </c>
+      <c r="F38" s="91">
+        <v>5</v>
+      </c>
+      <c r="G38" s="91">
+        <v>6</v>
+      </c>
+      <c r="H38" s="91">
+        <v>7</v>
+      </c>
+      <c r="I38" s="91">
+        <v>8</v>
+      </c>
+      <c r="J38" s="91">
+        <v>9</v>
+      </c>
+      <c r="K38" s="91">
+        <v>10</v>
+      </c>
+      <c r="L38" s="91">
+        <v>11</v>
+      </c>
+      <c r="M38" s="91">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="91" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="91" t="s">
+        <v>282</v>
+      </c>
+      <c r="E39" s="91" t="s">
+        <v>299</v>
+      </c>
+      <c r="F39" s="91"/>
+      <c r="G39" s="91"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="91"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="91" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" s="91" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="D40" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="E40" s="91" t="s">
+        <v>300</v>
+      </c>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="91"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="91"/>
+      <c r="K40" s="91"/>
+      <c r="L40" s="91"/>
+      <c r="M40" s="91"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="91" t="s">
+        <v>260</v>
+      </c>
+      <c r="D41" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="E41" s="91" t="s">
+        <v>301</v>
+      </c>
+      <c r="F41" s="91"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="91"/>
+      <c r="K41" s="91"/>
+      <c r="L41" s="91"/>
+      <c r="M41" s="91"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="91" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="D42" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="E42" s="91" t="s">
+        <v>302</v>
+      </c>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="91"/>
+      <c r="M42" s="91"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="D43" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="E43" s="91" t="s">
+        <v>303</v>
+      </c>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="91"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="D44" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="E44" s="91" t="s">
+        <v>304</v>
+      </c>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="91"/>
+      <c r="K44" s="91"/>
+      <c r="L44" s="91"/>
+      <c r="M44" s="91"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="E45" s="91"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="91"/>
+      <c r="K45" s="91"/>
+      <c r="L45" s="91"/>
+      <c r="M45" s="91"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="91" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="D46" s="91" t="s">
+        <v>298</v>
+      </c>
+      <c r="E46" s="91"/>
+      <c r="F46" s="91"/>
+      <c r="G46" s="91"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="91"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="56" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V3V4 16S sequences and MBDBS pipeline for oyster project
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E792D43-3E92-0948-BF22-A9D65DC2E519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E97303-9062-054C-8AD4-A61B67403699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5660" yWindow="460" windowWidth="27940" windowHeight="19560" firstSheet="4" activeTab="9" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
@@ -1332,7 +1332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1342,6 +1342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1571,7 +1577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1664,6 +1670,37 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1715,45 +1752,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2086,12 +2110,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2204,10 +2228,10 @@
       <c r="C9" s="61"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="90" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="75"/>
+      <c r="B13" s="90"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -2268,10 +2292,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="B32" s="75"/>
+      <c r="B32" s="90"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
@@ -2345,7 +2369,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2363,240 +2387,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="85" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="85" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" s="103" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="107" t="s">
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+    </row>
+    <row r="4" spans="1:15" s="86" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="87" t="s">
         <v>345</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="87" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="117" t="s">
         <v>368</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="87" t="s">
         <v>358</v>
       </c>
-      <c r="E4" s="107" t="s">
+      <c r="E4" s="87" t="s">
         <v>222</v>
       </c>
-      <c r="F4" s="107" t="s">
+      <c r="F4" s="87" t="s">
         <v>370</v>
       </c>
-      <c r="G4" s="108" t="s">
+      <c r="G4" s="87" t="s">
         <v>354</v>
       </c>
-      <c r="H4" s="101" t="s">
+      <c r="H4" s="118" t="s">
         <v>353</v>
       </c>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="87" t="s">
         <v>355</v>
       </c>
-      <c r="J4" s="108" t="s">
+      <c r="J4" s="87" t="s">
         <v>356</v>
       </c>
-      <c r="K4" s="101" t="s">
+      <c r="K4" s="118" t="s">
         <v>363</v>
       </c>
-      <c r="L4" s="108" t="s">
+      <c r="L4" s="87" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="109" t="s">
         <v>304</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="96" t="s">
+      <c r="H5" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I5" s="96" t="s">
+      <c r="I5" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J5" s="96" t="s">
+      <c r="J5" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="96" t="s">
+      <c r="K5" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L5" s="96" t="s">
+      <c r="L5" s="110" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="109" t="s">
         <v>308</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="109" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="96" t="s">
+      <c r="G6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="96" t="s">
+      <c r="H6" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I6" s="96" t="s">
+      <c r="I6" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J6" s="96" t="s">
+      <c r="J6" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="96" t="s">
+      <c r="K6" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="110" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="109" t="s">
         <v>310</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="109" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E7" s="95" t="s">
+      <c r="E7" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="96" t="s">
+      <c r="G7" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="96" t="s">
+      <c r="H7" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I7" s="96" t="s">
+      <c r="I7" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J7" s="96" t="s">
+      <c r="J7" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="96" t="s">
+      <c r="K7" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L7" s="96" t="s">
+      <c r="L7" s="110" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E8" s="95" t="s">
+      <c r="E8" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="96" t="s">
+      <c r="G8" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="96" t="s">
+      <c r="H8" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I8" s="96" t="s">
+      <c r="I8" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="96" t="s">
+      <c r="K8" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L8" s="96" t="s">
+      <c r="L8" s="110" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="109" t="s">
         <v>313</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="109" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E9" s="95" t="s">
+      <c r="E9" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="96" t="s">
+      <c r="H9" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I9" s="96" t="s">
+      <c r="I9" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J9" s="96" t="s">
+      <c r="J9" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="96" t="s">
+      <c r="K9" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L9" s="96" t="s">
+      <c r="L9" s="110" t="s">
         <v>367</v>
       </c>
       <c r="M9" s="2"/>
@@ -2604,40 +2632,40 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="109" t="s">
         <v>315</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="109" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="D10" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F10" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G10" s="96" t="s">
+      <c r="G10" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="96" t="s">
+      <c r="H10" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I10" s="96" t="s">
+      <c r="I10" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J10" s="96" t="s">
+      <c r="J10" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="96" t="s">
+      <c r="K10" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L10" s="96" t="s">
+      <c r="L10" s="110" t="s">
         <v>367</v>
       </c>
       <c r="M10" s="1"/>
@@ -2645,122 +2673,122 @@
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="109" t="s">
         <v>317</v>
       </c>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="109" t="s">
         <v>178</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E11" s="95" t="s">
+      <c r="E11" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F11" s="95" t="s">
+      <c r="F11" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G11" s="96" t="s">
+      <c r="G11" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="96" t="s">
+      <c r="H11" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I11" s="96" t="s">
+      <c r="I11" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J11" s="96" t="s">
+      <c r="J11" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="96" t="s">
+      <c r="K11" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L11" s="96" t="s">
+      <c r="L11" s="110" t="s">
         <v>367</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="95" t="s">
+    <row r="12" spans="1:15" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="109" t="s">
         <v>319</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="109" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E12" s="95" t="s">
+      <c r="E12" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F12" s="95" t="s">
+      <c r="F12" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G12" s="96" t="s">
+      <c r="G12" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="96" t="s">
+      <c r="H12" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I12" s="96" t="s">
+      <c r="I12" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J12" s="96" t="s">
+      <c r="J12" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="96" t="s">
+      <c r="K12" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L12" s="96" t="s">
+      <c r="L12" s="110" t="s">
         <v>367</v>
       </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="1"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="107"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="109" t="s">
         <v>321</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="109" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E13" s="95" t="s">
+      <c r="E13" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F13" s="95" t="s">
+      <c r="F13" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G13" s="96" t="s">
+      <c r="G13" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="96" t="s">
+      <c r="H13" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I13" s="96" t="s">
+      <c r="I13" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J13" s="96" t="s">
+      <c r="J13" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="96" t="s">
+      <c r="K13" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L13" s="96" t="s">
+      <c r="L13" s="110" t="s">
         <v>367</v>
       </c>
       <c r="M13" s="1"/>
@@ -2768,838 +2796,838 @@
       <c r="O13" s="62"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="109" t="s">
         <v>323</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="109" t="s">
         <v>257</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E14" s="95" t="s">
+      <c r="E14" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G14" s="96" t="s">
+      <c r="G14" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="96" t="s">
+      <c r="H14" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I14" s="96" t="s">
+      <c r="I14" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J14" s="96" t="s">
+      <c r="J14" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="96" t="s">
+      <c r="K14" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L14" s="96" t="s">
+      <c r="L14" s="110" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="95" t="s">
+      <c r="A15" s="109" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="109" t="s">
         <v>258</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D15" s="96" t="s">
+      <c r="D15" s="110" t="s">
         <v>359</v>
       </c>
-      <c r="E15" s="95" t="s">
+      <c r="E15" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F15" s="95" t="s">
+      <c r="F15" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G15" s="96" t="s">
+      <c r="G15" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="96" t="s">
+      <c r="H15" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="I15" s="96" t="s">
+      <c r="I15" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="96" t="s">
+      <c r="K15" s="110" t="s">
         <v>366</v>
       </c>
-      <c r="L15" s="96" t="s">
+      <c r="L15" s="110" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="109" t="s">
         <v>327</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="119" t="s">
         <v>259</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="C16" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D16" s="106" t="s">
+      <c r="D16" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E16" s="95" t="s">
+      <c r="E16" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G16" s="96" t="s">
+      <c r="G16" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="104" t="s">
+      <c r="H16" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="109" t="s">
         <v>328</v>
       </c>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="119" t="s">
         <v>260</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D17" s="106" t="s">
+      <c r="D17" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E17" s="95" t="s">
+      <c r="E17" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F17" s="95" t="s">
+      <c r="F17" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G17" s="96" t="s">
+      <c r="G17" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="104" t="s">
+      <c r="H17" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="96" t="s">
+      <c r="I17" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="96" t="s">
+      <c r="J17" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="96" t="s">
+      <c r="K17" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="96" t="s">
+      <c r="L17" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="95" t="s">
+      <c r="A18" s="109" t="s">
         <v>329</v>
       </c>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="119" t="s">
         <v>261</v>
       </c>
-      <c r="C18" s="106" t="s">
+      <c r="C18" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D18" s="106" t="s">
+      <c r="D18" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E18" s="95" t="s">
+      <c r="E18" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F18" s="95" t="s">
+      <c r="F18" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G18" s="96" t="s">
+      <c r="G18" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="104" t="s">
+      <c r="H18" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="96" t="s">
+      <c r="I18" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="96" t="s">
+      <c r="J18" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="96" t="s">
+      <c r="K18" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="96" t="s">
+      <c r="L18" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="109" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="119" t="s">
         <v>262</v>
       </c>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D19" s="106" t="s">
+      <c r="D19" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E19" s="95" t="s">
+      <c r="E19" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F19" s="95" t="s">
+      <c r="F19" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G19" s="96" t="s">
+      <c r="G19" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="104" t="s">
+      <c r="H19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="96" t="s">
+      <c r="J19" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="96" t="s">
+      <c r="K19" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="96" t="s">
+      <c r="L19" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="95" t="s">
+      <c r="A20" s="109" t="s">
         <v>331</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="119" t="s">
         <v>279</v>
       </c>
-      <c r="C20" s="106" t="s">
+      <c r="C20" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D20" s="106" t="s">
+      <c r="D20" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E20" s="95" t="s">
+      <c r="E20" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="95" t="s">
+      <c r="F20" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G20" s="96" t="s">
+      <c r="G20" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="104" t="s">
+      <c r="H20" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="96" t="s">
+      <c r="I20" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="96" t="s">
+      <c r="J20" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="96" t="s">
+      <c r="K20" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="96" t="s">
+      <c r="L20" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="109" t="s">
         <v>332</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="119" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D21" s="106" t="s">
+      <c r="D21" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E21" s="95" t="s">
+      <c r="E21" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G21" s="96" t="s">
+      <c r="G21" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="104" t="s">
+      <c r="H21" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="96" t="s">
+      <c r="I21" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="96" t="s">
+      <c r="J21" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K21" s="96" t="s">
+      <c r="K21" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="96" t="s">
+      <c r="L21" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="119" t="s">
         <v>285</v>
       </c>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D22" s="106" t="s">
+      <c r="D22" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E22" s="95" t="s">
+      <c r="E22" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F22" s="95" t="s">
+      <c r="F22" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G22" s="96" t="s">
+      <c r="G22" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="104" t="s">
+      <c r="H22" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="96" t="s">
+      <c r="I22" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="96" t="s">
+      <c r="K22" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L22" s="96" t="s">
+      <c r="L22" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="109" t="s">
         <v>333</v>
       </c>
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="119" t="s">
         <v>286</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C23" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D23" s="106" t="s">
+      <c r="D23" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E23" s="95" t="s">
+      <c r="E23" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F23" s="95" t="s">
+      <c r="F23" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G23" s="96" t="s">
+      <c r="G23" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="104" t="s">
+      <c r="H23" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="96" t="s">
+      <c r="I23" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="96" t="s">
+      <c r="J23" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="96" t="s">
+      <c r="K23" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L23" s="96" t="s">
+      <c r="L23" s="110" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="95" t="s">
+    <row r="24" spans="1:12" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="109" t="s">
         <v>334</v>
       </c>
-      <c r="B24" s="106" t="s">
+      <c r="B24" s="119" t="s">
         <v>292</v>
       </c>
-      <c r="C24" s="106" t="s">
+      <c r="C24" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D24" s="106" t="s">
+      <c r="D24" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="E24" s="95" t="s">
+      <c r="E24" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G24" s="96" t="s">
+      <c r="G24" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="105" t="s">
+      <c r="H24" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="I24" s="96" t="s">
+      <c r="I24" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="J24" s="96" t="s">
+      <c r="J24" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K24" s="96" t="s">
+      <c r="K24" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="96" t="s">
+      <c r="L24" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="95" t="s">
+      <c r="A25" s="109" t="s">
         <v>335</v>
       </c>
-      <c r="B25" s="106" t="s">
+      <c r="B25" s="119" t="s">
         <v>293</v>
       </c>
-      <c r="C25" s="106" t="s">
+      <c r="C25" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D25" s="106" t="s">
+      <c r="D25" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="E25" s="95" t="s">
+      <c r="E25" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F25" s="95" t="s">
+      <c r="F25" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G25" s="96" t="s">
+      <c r="G25" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="105" t="s">
+      <c r="H25" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="I25" s="96" t="s">
+      <c r="I25" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="J25" s="96" t="s">
+      <c r="J25" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K25" s="96" t="s">
+      <c r="K25" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="96" t="s">
+      <c r="L25" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="109" t="s">
         <v>336</v>
       </c>
-      <c r="B26" s="106" t="s">
+      <c r="B26" s="119" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D26" s="106" t="s">
+      <c r="D26" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F26" s="95" t="s">
+      <c r="F26" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G26" s="96" t="s">
+      <c r="G26" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="105" t="s">
+      <c r="H26" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="I26" s="96" t="s">
+      <c r="I26" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="J26" s="96" t="s">
+      <c r="J26" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K26" s="96" t="s">
+      <c r="K26" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L26" s="96" t="s">
+      <c r="L26" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="109" t="s">
         <v>337</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="119" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D27" s="106" t="s">
+      <c r="D27" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="E27" s="95" t="s">
+      <c r="E27" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F27" s="95" t="s">
+      <c r="F27" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G27" s="96" t="s">
+      <c r="G27" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="105" t="s">
+      <c r="H27" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="I27" s="96" t="s">
+      <c r="I27" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="J27" s="96" t="s">
+      <c r="J27" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K27" s="96" t="s">
+      <c r="K27" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L27" s="96" t="s">
+      <c r="L27" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="95" t="s">
+      <c r="A28" s="109" t="s">
         <v>338</v>
       </c>
-      <c r="B28" s="106" t="s">
+      <c r="B28" s="119" t="s">
         <v>296</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D28" s="106" t="s">
+      <c r="D28" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="E28" s="95" t="s">
+      <c r="E28" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F28" s="95" t="s">
+      <c r="F28" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G28" s="96" t="s">
+      <c r="G28" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="105" t="s">
+      <c r="H28" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="I28" s="96" t="s">
+      <c r="I28" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="J28" s="96" t="s">
+      <c r="J28" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="96" t="s">
+      <c r="K28" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="96" t="s">
+      <c r="L28" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="95" t="s">
+      <c r="A29" s="109" t="s">
         <v>339</v>
       </c>
-      <c r="B29" s="106" t="s">
+      <c r="B29" s="119" t="s">
         <v>297</v>
       </c>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="D29" s="106" t="s">
+      <c r="D29" s="119" t="s">
         <v>362</v>
       </c>
-      <c r="E29" s="95" t="s">
+      <c r="E29" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F29" s="95" t="s">
+      <c r="F29" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G29" s="96" t="s">
+      <c r="G29" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="105" t="s">
+      <c r="H29" s="121" t="s">
         <v>349</v>
       </c>
-      <c r="I29" s="105" t="s">
+      <c r="I29" s="121" t="s">
         <v>350</v>
       </c>
-      <c r="J29" s="96" t="s">
+      <c r="J29" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K29" s="96" t="s">
+      <c r="K29" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L29" s="96" t="s">
+      <c r="L29" s="110" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="95" t="s">
+    <row r="30" spans="1:12" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="109" t="s">
         <v>340</v>
       </c>
-      <c r="B30" s="106" t="s">
+      <c r="B30" s="119" t="s">
         <v>298</v>
       </c>
-      <c r="C30" s="106" t="s">
+      <c r="C30" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="D30" s="106" t="s">
+      <c r="D30" s="119" t="s">
         <v>362</v>
       </c>
-      <c r="E30" s="95" t="s">
+      <c r="E30" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F30" s="95" t="s">
+      <c r="F30" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G30" s="96" t="s">
+      <c r="G30" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="105" t="s">
+      <c r="H30" s="121" t="s">
         <v>349</v>
       </c>
-      <c r="I30" s="105" t="s">
+      <c r="I30" s="121" t="s">
         <v>350</v>
       </c>
-      <c r="J30" s="96" t="s">
+      <c r="J30" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K30" s="96" t="s">
+      <c r="K30" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L30" s="96" t="s">
+      <c r="L30" s="110" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="95" t="s">
+    <row r="31" spans="1:12" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="109" t="s">
         <v>341</v>
       </c>
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="119" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="106" t="s">
+      <c r="C31" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="D31" s="106" t="s">
+      <c r="D31" s="119" t="s">
         <v>362</v>
       </c>
-      <c r="E31" s="95" t="s">
+      <c r="E31" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F31" s="95" t="s">
+      <c r="F31" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G31" s="96" t="s">
+      <c r="G31" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="105" t="s">
+      <c r="H31" s="121" t="s">
         <v>349</v>
       </c>
-      <c r="I31" s="105" t="s">
+      <c r="I31" s="121" t="s">
         <v>350</v>
       </c>
-      <c r="J31" s="96" t="s">
+      <c r="J31" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K31" s="96" t="s">
+      <c r="K31" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L31" s="96" t="s">
+      <c r="L31" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="95" t="s">
+      <c r="A32" s="109" t="s">
         <v>342</v>
       </c>
-      <c r="B32" s="106" t="s">
+      <c r="B32" s="119" t="s">
         <v>300</v>
       </c>
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D32" s="106" t="s">
+      <c r="D32" s="119" t="s">
         <v>360</v>
       </c>
-      <c r="E32" s="95" t="s">
+      <c r="E32" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F32" s="95" t="s">
+      <c r="F32" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G32" s="96" t="s">
+      <c r="G32" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="104" t="s">
+      <c r="H32" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="96" t="s">
+      <c r="I32" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="96" t="s">
+      <c r="J32" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K32" s="96" t="s">
+      <c r="K32" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L32" s="96" t="s">
+      <c r="L32" s="110" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="95" t="s">
+    <row r="33" spans="1:12" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="109" t="s">
         <v>343</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="119" t="s">
         <v>301</v>
       </c>
-      <c r="C33" s="106" t="s">
+      <c r="C33" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D33" s="106" t="s">
+      <c r="D33" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="E33" s="95" t="s">
+      <c r="E33" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F33" s="95" t="s">
+      <c r="F33" s="109" t="s">
         <v>372</v>
       </c>
-      <c r="G33" s="96" t="s">
+      <c r="G33" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="105" t="s">
+      <c r="H33" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="I33" s="96" t="s">
+      <c r="I33" s="110" t="s">
         <v>188</v>
       </c>
-      <c r="J33" s="96" t="s">
+      <c r="J33" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K33" s="96" t="s">
+      <c r="K33" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L33" s="96" t="s">
+      <c r="L33" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="95" t="s">
+      <c r="A34" s="109" t="s">
         <v>344</v>
       </c>
-      <c r="B34" s="106" t="s">
+      <c r="B34" s="119" t="s">
         <v>302</v>
       </c>
-      <c r="C34" s="106" t="s">
+      <c r="C34" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="D34" s="106" t="s">
+      <c r="D34" s="119" t="s">
         <v>362</v>
       </c>
-      <c r="E34" s="95" t="s">
+      <c r="E34" s="109" t="s">
         <v>223</v>
       </c>
-      <c r="F34" s="95" t="s">
+      <c r="F34" s="109" t="s">
         <v>371</v>
       </c>
-      <c r="G34" s="96" t="s">
+      <c r="G34" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="105" t="s">
+      <c r="H34" s="121" t="s">
         <v>349</v>
       </c>
-      <c r="I34" s="105" t="s">
+      <c r="I34" s="121" t="s">
         <v>350</v>
       </c>
-      <c r="J34" s="96" t="s">
+      <c r="J34" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="96" t="s">
+      <c r="K34" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L34" s="96" t="s">
+      <c r="L34" s="110" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="88" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="91"/>
-      <c r="B37" s="91">
+      <c r="A37" s="74"/>
+      <c r="B37" s="74">
         <v>1</v>
       </c>
-      <c r="C37" s="91">
+      <c r="C37" s="74">
         <v>2</v>
       </c>
-      <c r="D37" s="91">
+      <c r="D37" s="74">
         <v>3</v>
       </c>
-      <c r="E37" s="91">
+      <c r="E37" s="74">
         <v>4</v>
       </c>
       <c r="F37" s="59"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="91" t="s">
+      <c r="C38" s="74" t="s">
         <v>256</v>
       </c>
-      <c r="D38" s="91" t="s">
+      <c r="D38" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="E38" s="91" t="s">
+      <c r="E38" s="74" t="s">
         <v>297</v>
       </c>
       <c r="F38" s="59"/>
@@ -3609,19 +3637,19 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="C39" s="91" t="s">
+      <c r="C39" s="74" t="s">
         <v>257</v>
       </c>
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="74" t="s">
         <v>285</v>
       </c>
-      <c r="E39" s="91" t="s">
+      <c r="E39" s="74" t="s">
         <v>298</v>
       </c>
       <c r="F39" s="59"/>
@@ -3631,19 +3659,19 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="C40" s="91" t="s">
+      <c r="C40" s="74" t="s">
         <v>258</v>
       </c>
-      <c r="D40" s="91" t="s">
+      <c r="D40" s="74" t="s">
         <v>286</v>
       </c>
-      <c r="E40" s="91" t="s">
+      <c r="E40" s="74" t="s">
         <v>299</v>
       </c>
       <c r="F40" s="59"/>
@@ -3653,19 +3681,19 @@
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="91" t="s">
+      <c r="A41" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="91" t="s">
+      <c r="C41" s="74" t="s">
         <v>259</v>
       </c>
-      <c r="D41" s="91" t="s">
+      <c r="D41" s="74" t="s">
         <v>292</v>
       </c>
-      <c r="E41" s="91" t="s">
+      <c r="E41" s="74" t="s">
         <v>300</v>
       </c>
       <c r="F41" s="59"/>
@@ -3675,19 +3703,19 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="91" t="s">
+      <c r="B42" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="C42" s="91" t="s">
+      <c r="C42" s="74" t="s">
         <v>260</v>
       </c>
-      <c r="D42" s="91" t="s">
+      <c r="D42" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="E42" s="91" t="s">
+      <c r="E42" s="74" t="s">
         <v>301</v>
       </c>
       <c r="F42" s="59"/>
@@ -3697,56 +3725,59 @@
       <c r="J42" s="62"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="91" t="s">
+      <c r="A43" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="91" t="s">
+      <c r="C43" s="74" t="s">
         <v>261</v>
       </c>
-      <c r="D43" s="91" t="s">
+      <c r="D43" s="74" t="s">
         <v>294</v>
       </c>
-      <c r="E43" s="91" t="s">
+      <c r="E43" s="74" t="s">
         <v>302</v>
       </c>
       <c r="F43" s="59"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="91" t="s">
+      <c r="A44" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="91" t="s">
+      <c r="B44" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="C44" s="91" t="s">
+      <c r="C44" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="D44" s="91" t="s">
+      <c r="D44" s="74" t="s">
         <v>295</v>
       </c>
-      <c r="E44" s="91"/>
+      <c r="E44" s="74"/>
       <c r="F44" s="59"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="91" t="s">
+      <c r="A45" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="C45" s="91" t="s">
+      <c r="C45" s="74" t="s">
         <v>279</v>
       </c>
-      <c r="D45" s="91" t="s">
+      <c r="D45" s="74" t="s">
         <v>296</v>
       </c>
-      <c r="E45" s="91"/>
+      <c r="E45" s="74"/>
       <c r="F45" s="59"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:G2"/>
+  </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3795,7 +3826,7 @@
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="91" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3806,7 +3837,7 @@
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="91"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -3815,7 +3846,7 @@
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="76"/>
+      <c r="C5" s="91"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -3861,20 +3892,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -3905,16 +3936,16 @@
         <v>85</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -4331,12 +4362,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
       <c r="K16" s="5">
         <v>1</v>
       </c>
@@ -4485,12 +4516,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
       <c r="K24" s="5">
         <v>1</v>
       </c>
@@ -4694,32 +4725,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
@@ -5080,12 +5111,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -5135,12 +5166,12 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -5236,16 +5267,16 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="79"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
@@ -5440,17 +5471,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -5734,12 +5765,12 @@
       <c r="M13" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
@@ -6163,39 +6194,39 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="98" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="99"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="100"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="86" t="s">
+      <c r="B34" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="88"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="103"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
       <c r="F37" s="55" t="s">
         <v>159</v>
       </c>
@@ -6341,29 +6372,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="88"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="103"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -6621,12 +6652,12 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
       <c r="F27" s="55" t="s">
         <v>159</v>
       </c>
@@ -6774,26 +6805,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="105" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -7189,17 +7220,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="104" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -7511,8 +7542,8 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:E46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7535,1441 +7566,1455 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="104" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
     </row>
     <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>182</v>
       </c>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
     </row>
     <row r="4" spans="1:17" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="77" t="s">
         <v>289</v>
       </c>
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="83" t="s">
         <v>290</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="84" t="s">
         <v>266</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="84" t="s">
         <v>233</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="H4" s="94" t="s">
+      <c r="H4" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="94" t="s">
+      <c r="I4" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="100" t="s">
+      <c r="K4" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="L4" s="101" t="s">
+      <c r="L4" s="84" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="78" t="s">
         <v>304</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E5" s="96" t="s">
+      <c r="E5" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G5" s="95">
+      <c r="G5" s="78">
         <v>12</v>
       </c>
-      <c r="H5" s="95" t="s">
+      <c r="H5" s="78" t="s">
         <v>307</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="95">
+      <c r="J5" s="78">
         <v>20220321</v>
       </c>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="93"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="76"/>
       <c r="O5" s="58"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="78" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E6" s="96" t="s">
+      <c r="E6" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G6" s="95">
+      <c r="G6" s="78">
         <v>72</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="I6" s="95" t="s">
+      <c r="I6" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="95">
+      <c r="J6" s="78">
         <v>20220321</v>
       </c>
-      <c r="K6" s="97"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="93"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="76"/>
       <c r="O6" s="58"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="78" t="s">
         <v>310</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G7" s="95">
+      <c r="G7" s="78">
         <v>78</v>
       </c>
-      <c r="H7" s="95" t="s">
+      <c r="H7" s="78" t="s">
         <v>311</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="95">
+      <c r="J7" s="78">
         <v>20220321</v>
       </c>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="93"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="76"/>
       <c r="O7" s="58"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="78" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E8" s="96" t="s">
+      <c r="E8" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G8" s="95">
+      <c r="G8" s="78">
         <v>84</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="78" t="s">
         <v>312</v>
       </c>
-      <c r="I8" s="95" t="s">
+      <c r="I8" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="95">
+      <c r="J8" s="78">
         <v>20220321</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="93"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="76"/>
       <c r="O8" s="58"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="78" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E9" s="96" t="s">
+      <c r="E9" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G9" s="95">
+      <c r="G9" s="78">
         <v>120</v>
       </c>
-      <c r="H9" s="95" t="s">
+      <c r="H9" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="I9" s="95" t="s">
+      <c r="I9" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="95">
+      <c r="J9" s="78">
         <v>20220321</v>
       </c>
-      <c r="K9" s="97"/>
-      <c r="L9" s="97"/>
-      <c r="M9" s="93"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="76"/>
       <c r="O9" s="58"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="78" t="s">
         <v>177</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E10" s="96" t="s">
+      <c r="E10" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F10" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G10" s="95">
+      <c r="G10" s="78">
         <v>132</v>
       </c>
-      <c r="H10" s="95" t="s">
+      <c r="H10" s="78" t="s">
         <v>316</v>
       </c>
-      <c r="I10" s="95" t="s">
+      <c r="I10" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="95">
+      <c r="J10" s="78">
         <v>20220321</v>
       </c>
-      <c r="K10" s="97"/>
-      <c r="L10" s="97"/>
-      <c r="M10" s="93"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="76"/>
       <c r="O10" s="58"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E11" s="96" t="s">
+      <c r="E11" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F11" s="95" t="s">
+      <c r="F11" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G11" s="95">
+      <c r="G11" s="78">
         <v>138</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="78" t="s">
         <v>318</v>
       </c>
-      <c r="I11" s="95" t="s">
+      <c r="I11" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="95">
+      <c r="J11" s="78">
         <v>20220321</v>
       </c>
-      <c r="K11" s="97"/>
-      <c r="L11" s="97"/>
-      <c r="M11" s="93"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="76"/>
       <c r="O11" s="58"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="95" t="s">
+    <row r="12" spans="1:17" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="109" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="109" t="s">
         <v>319</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="109" t="s">
         <v>303</v>
       </c>
-      <c r="E12" s="96" t="s">
+      <c r="E12" s="110" t="s">
         <v>305</v>
       </c>
-      <c r="F12" s="95" t="s">
+      <c r="F12" s="109" t="s">
         <v>306</v>
       </c>
-      <c r="G12" s="95">
+      <c r="G12" s="109">
         <v>144</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="109" t="s">
         <v>320</v>
       </c>
-      <c r="I12" s="95" t="s">
+      <c r="I12" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="95">
+      <c r="J12" s="109">
         <v>20220321</v>
       </c>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="93"/>
-      <c r="O12" s="58"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
+      <c r="O12" s="113"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="78" t="s">
         <v>321</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E13" s="96" t="s">
+      <c r="E13" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F13" s="95" t="s">
+      <c r="F13" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G13" s="95">
+      <c r="G13" s="78">
         <v>168</v>
       </c>
-      <c r="H13" s="95" t="s">
+      <c r="H13" s="78" t="s">
         <v>322</v>
       </c>
-      <c r="I13" s="95" t="s">
+      <c r="I13" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="95">
+      <c r="J13" s="78">
         <v>20220321</v>
       </c>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="93"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="76"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="78" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G14" s="95">
+      <c r="G14" s="78">
         <v>204</v>
       </c>
-      <c r="H14" s="95" t="s">
+      <c r="H14" s="78" t="s">
         <v>324</v>
       </c>
-      <c r="I14" s="95" t="s">
+      <c r="I14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="95">
+      <c r="J14" s="78">
         <v>20220321</v>
       </c>
-      <c r="K14" s="97"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="93"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="76"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="95" t="s">
+      <c r="A15" s="78" t="s">
         <v>258</v>
       </c>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="78" t="s">
         <v>325</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E15" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="F15" s="95" t="s">
+      <c r="F15" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="G15" s="95">
+      <c r="G15" s="78">
         <v>210</v>
       </c>
-      <c r="H15" s="95" t="s">
+      <c r="H15" s="78" t="s">
         <v>326</v>
       </c>
-      <c r="I15" s="95" t="s">
+      <c r="I15" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="95">
+      <c r="J15" s="78">
         <v>20220321</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="93"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="76"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="74" t="s">
         <v>259</v>
       </c>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C16" s="91" t="s">
+      <c r="C16" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D16" s="91" t="s">
+      <c r="D16" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E16" s="91" t="s">
+      <c r="E16" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F16" s="91" t="s">
+      <c r="F16" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G16" s="98" t="s">
+      <c r="G16" s="81" t="s">
         <v>255</v>
       </c>
-      <c r="H16" s="91" t="s">
+      <c r="H16" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="J16" s="91" t="s">
+      <c r="J16" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="K16" s="91">
+      <c r="K16" s="74">
         <v>3</v>
       </c>
-      <c r="L16" s="91">
+      <c r="L16" s="74">
         <f>70-25</f>
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="91" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="74" t="s">
         <v>260</v>
       </c>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="C17" s="91" t="s">
+      <c r="C17" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D17" s="91" t="s">
+      <c r="D17" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E17" s="91" t="s">
+      <c r="E17" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F17" s="91" t="s">
+      <c r="F17" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G17" s="91" t="s">
+      <c r="G17" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="H17" s="91" t="s">
+      <c r="H17" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I17" s="91" t="s">
+      <c r="I17" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="J17" s="91" t="s">
+      <c r="J17" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="K17" s="91">
+      <c r="K17" s="74">
         <v>3</v>
       </c>
-      <c r="L17" s="91">
+      <c r="L17" s="74">
         <f>70-25</f>
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="91" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="74" t="s">
         <v>261</v>
       </c>
-      <c r="B18" s="95" t="s">
+      <c r="B18" s="78" t="s">
         <v>329</v>
       </c>
-      <c r="C18" s="91" t="s">
+      <c r="C18" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D18" s="91" t="s">
+      <c r="D18" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E18" s="91" t="s">
+      <c r="E18" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F18" s="91" t="s">
+      <c r="F18" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G18" s="91" t="s">
+      <c r="G18" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="H18" s="91" t="s">
+      <c r="H18" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I18" s="91" t="s">
+      <c r="I18" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="J18" s="91" t="s">
+      <c r="J18" s="74" t="s">
         <v>269</v>
       </c>
-      <c r="K18" s="91">
+      <c r="K18" s="74">
         <v>3</v>
       </c>
-      <c r="L18" s="91">
+      <c r="L18" s="74">
         <f>70-25</f>
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="91" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="91" t="s">
+      <c r="D19" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E19" s="91" t="s">
+      <c r="E19" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F19" s="91" t="s">
+      <c r="F19" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G19" s="91" t="s">
+      <c r="G19" s="74" t="s">
         <v>270</v>
       </c>
-      <c r="H19" s="99" t="s">
+      <c r="H19" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="I19" s="99" t="s">
+      <c r="I19" s="82" t="s">
         <v>287</v>
       </c>
-      <c r="J19" s="91" t="s">
+      <c r="J19" s="74" t="s">
         <v>271</v>
       </c>
-      <c r="K19" s="91">
+      <c r="K19" s="74">
         <v>2</v>
       </c>
-      <c r="L19" s="91">
+      <c r="L19" s="74">
         <f>45-25</f>
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="91" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="74" t="s">
         <v>279</v>
       </c>
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="78" t="s">
         <v>331</v>
       </c>
-      <c r="C20" s="91" t="s">
+      <c r="C20" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D20" s="91" t="s">
+      <c r="D20" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E20" s="91" t="s">
+      <c r="E20" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F20" s="91" t="s">
+      <c r="F20" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G20" s="91" t="s">
+      <c r="G20" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="H20" s="99" t="s">
+      <c r="H20" s="82" t="s">
         <v>278</v>
       </c>
-      <c r="I20" s="99" t="s">
+      <c r="I20" s="82" t="s">
         <v>288</v>
       </c>
-      <c r="J20" s="91" t="s">
+      <c r="J20" s="74" t="s">
         <v>271</v>
       </c>
-      <c r="K20" s="91">
+      <c r="K20" s="74">
         <v>2</v>
       </c>
-      <c r="L20" s="91">
+      <c r="L20" s="74">
         <f>45-25</f>
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="91" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="B21" s="95" t="s">
+      <c r="B21" s="78" t="s">
         <v>332</v>
       </c>
-      <c r="C21" s="91" t="s">
+      <c r="C21" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D21" s="91" t="s">
+      <c r="D21" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E21" s="91" t="s">
+      <c r="E21" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F21" s="98" t="s">
+      <c r="F21" s="81" t="s">
         <v>272</v>
       </c>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="81" t="s">
         <v>255</v>
       </c>
-      <c r="H21" s="99" t="s">
+      <c r="H21" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="I21" s="99" t="s">
+      <c r="I21" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="J21" s="91" t="s">
+      <c r="J21" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="K21" s="91">
+      <c r="K21" s="74">
         <v>3</v>
       </c>
-      <c r="L21" s="91">
+      <c r="L21" s="74">
         <f t="shared" ref="L21:L34" si="0">70-25</f>
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="91" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="74" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="91" t="s">
+      <c r="C22" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D22" s="91" t="s">
+      <c r="D22" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E22" s="91" t="s">
+      <c r="E22" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F22" s="98" t="s">
+      <c r="F22" s="81" t="s">
         <v>272</v>
       </c>
-      <c r="G22" s="91" t="s">
+      <c r="G22" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="H22" s="99" t="s">
+      <c r="H22" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="I22" s="99" t="s">
+      <c r="I22" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="J22" s="99" t="s">
+      <c r="J22" s="82" t="s">
         <v>264</v>
       </c>
-      <c r="K22" s="91">
+      <c r="K22" s="74">
         <v>3</v>
       </c>
-      <c r="L22" s="91">
+      <c r="L22" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="91" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="74" t="s">
         <v>286</v>
       </c>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C23" s="91" t="s">
+      <c r="C23" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D23" s="91" t="s">
+      <c r="D23" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F23" s="98" t="s">
+      <c r="F23" s="81" t="s">
         <v>272</v>
       </c>
-      <c r="G23" s="91" t="s">
+      <c r="G23" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="H23" s="99" t="s">
+      <c r="H23" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="I23" s="99" t="s">
+      <c r="I23" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="J23" s="99" t="s">
+      <c r="J23" s="82" t="s">
         <v>271</v>
       </c>
-      <c r="K23" s="91">
+      <c r="K23" s="74">
         <v>3</v>
       </c>
-      <c r="L23" s="91">
+      <c r="L23" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="91" t="s">
+    <row r="24" spans="1:14" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="82" t="s">
         <v>292</v>
       </c>
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="109" t="s">
         <v>334</v>
       </c>
-      <c r="C24" s="91" t="s">
+      <c r="C24" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="D24" s="91" t="s">
+      <c r="D24" s="82" t="s">
         <v>265</v>
       </c>
-      <c r="E24" s="91" t="s">
+      <c r="E24" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="F24" s="91" t="s">
+      <c r="F24" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="G24" s="91" t="s">
+      <c r="G24" s="82" t="s">
         <v>255</v>
       </c>
-      <c r="H24" s="91" t="s">
+      <c r="H24" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="I24" s="91" t="s">
+      <c r="I24" s="82" t="s">
         <v>276</v>
       </c>
-      <c r="J24" s="91" t="s">
+      <c r="J24" s="82" t="s">
         <v>264</v>
       </c>
-      <c r="K24" s="91">
+      <c r="K24" s="82">
         <v>3</v>
       </c>
-      <c r="L24" s="91">
+      <c r="L24" s="82">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="91" t="s">
+      <c r="M24" s="113"/>
+      <c r="N24" s="113"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="78" t="s">
         <v>335</v>
       </c>
-      <c r="C25" s="91" t="s">
+      <c r="C25" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D25" s="91" t="s">
+      <c r="D25" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E25" s="91" t="s">
+      <c r="E25" s="74" t="s">
         <v>274</v>
       </c>
-      <c r="F25" s="91" t="s">
+      <c r="F25" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G25" s="91" t="s">
+      <c r="G25" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="H25" s="91" t="s">
+      <c r="H25" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I25" s="91" t="s">
+      <c r="I25" s="74" t="s">
         <v>276</v>
       </c>
-      <c r="J25" s="91" t="s">
+      <c r="J25" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="K25" s="91">
+      <c r="K25" s="74">
         <v>3</v>
       </c>
-      <c r="L25" s="91">
+      <c r="L25" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="91" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="74" t="s">
         <v>294</v>
       </c>
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="78" t="s">
         <v>336</v>
       </c>
-      <c r="C26" s="91" t="s">
+      <c r="C26" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D26" s="91" t="s">
+      <c r="D26" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="74" t="s">
         <v>274</v>
       </c>
-      <c r="F26" s="91" t="s">
+      <c r="F26" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G26" s="91" t="s">
+      <c r="G26" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="H26" s="91" t="s">
+      <c r="H26" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I26" s="91" t="s">
+      <c r="I26" s="74" t="s">
         <v>276</v>
       </c>
-      <c r="J26" s="91" t="s">
+      <c r="J26" s="74" t="s">
         <v>271</v>
       </c>
-      <c r="K26" s="91">
+      <c r="K26" s="74">
         <v>3</v>
       </c>
-      <c r="L26" s="91">
+      <c r="L26" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="91" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="74" t="s">
         <v>295</v>
       </c>
-      <c r="B27" s="95" t="s">
+      <c r="B27" s="78" t="s">
         <v>337</v>
       </c>
-      <c r="C27" s="91" t="s">
+      <c r="C27" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D27" s="91" t="s">
+      <c r="D27" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E27" s="91" t="s">
+      <c r="E27" s="74" t="s">
         <v>274</v>
       </c>
-      <c r="F27" s="91" t="s">
+      <c r="F27" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G27" s="91" t="s">
+      <c r="G27" s="74" t="s">
         <v>275</v>
       </c>
-      <c r="H27" s="91" t="s">
+      <c r="H27" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I27" s="91" t="s">
+      <c r="I27" s="74" t="s">
         <v>276</v>
       </c>
-      <c r="J27" s="91" t="s">
+      <c r="J27" s="74" t="s">
         <v>271</v>
       </c>
-      <c r="K27" s="91">
+      <c r="K27" s="74">
         <v>3</v>
       </c>
-      <c r="L27" s="91">
+      <c r="L27" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="91" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="74" t="s">
         <v>296</v>
       </c>
-      <c r="B28" s="95" t="s">
+      <c r="B28" s="78" t="s">
         <v>338</v>
       </c>
-      <c r="C28" s="91" t="s">
+      <c r="C28" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D28" s="91" t="s">
+      <c r="D28" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E28" s="91" t="s">
+      <c r="E28" s="74" t="s">
         <v>274</v>
       </c>
-      <c r="F28" s="91" t="s">
+      <c r="F28" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G28" s="91" t="s">
+      <c r="G28" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="H28" s="99" t="s">
+      <c r="H28" s="82" t="s">
         <v>278</v>
       </c>
-      <c r="I28" s="91" t="s">
+      <c r="I28" s="74" t="s">
         <v>276</v>
       </c>
-      <c r="J28" s="91" t="s">
+      <c r="J28" s="74" t="s">
         <v>277</v>
       </c>
-      <c r="K28" s="91">
+      <c r="K28" s="74">
         <v>3</v>
       </c>
-      <c r="L28" s="91">
+      <c r="L28" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="91" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="74" t="s">
         <v>297</v>
       </c>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="78" t="s">
         <v>339</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="74" t="s">
         <v>281</v>
       </c>
-      <c r="E29" s="91" t="s">
+      <c r="E29" s="74" t="s">
         <v>282</v>
       </c>
-      <c r="F29" s="91" t="s">
+      <c r="F29" s="74" t="s">
         <v>272</v>
       </c>
-      <c r="G29" s="91" t="s">
+      <c r="G29" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="91" t="s">
+      <c r="H29" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="I29" s="91" t="s">
+      <c r="I29" s="74" t="s">
         <v>283</v>
       </c>
-      <c r="J29" s="91" t="s">
+      <c r="J29" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="K29" s="91">
+      <c r="K29" s="74">
         <v>3</v>
       </c>
-      <c r="L29" s="91">
+      <c r="L29" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="91" t="s">
+    <row r="30" spans="1:14" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="82" t="s">
         <v>298</v>
       </c>
-      <c r="B30" s="95" t="s">
+      <c r="B30" s="109" t="s">
         <v>340</v>
       </c>
-      <c r="C30" s="91" t="s">
+      <c r="C30" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="D30" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="E30" s="91" t="s">
+      <c r="E30" s="82" t="s">
         <v>282</v>
       </c>
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="G30" s="91" t="s">
+      <c r="G30" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="H30" s="91" t="s">
+      <c r="H30" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="I30" s="91" t="s">
+      <c r="I30" s="82" t="s">
         <v>283</v>
       </c>
-      <c r="J30" s="91" t="s">
+      <c r="J30" s="82" t="s">
         <v>264</v>
       </c>
-      <c r="K30" s="91">
+      <c r="K30" s="82">
         <v>3</v>
       </c>
-      <c r="L30" s="91">
+      <c r="L30" s="82">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="91" t="s">
+      <c r="M30" s="113"/>
+      <c r="N30" s="113"/>
+    </row>
+    <row r="31" spans="1:14" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="82" t="s">
         <v>299</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="109" t="s">
         <v>341</v>
       </c>
-      <c r="C31" s="91" t="s">
+      <c r="C31" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="E31" s="91" t="s">
+      <c r="E31" s="82" t="s">
         <v>282</v>
       </c>
-      <c r="F31" s="91" t="s">
+      <c r="F31" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="G31" s="91" t="s">
+      <c r="G31" s="82" t="s">
         <v>268</v>
       </c>
-      <c r="H31" s="91" t="s">
+      <c r="H31" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="I31" s="91" t="s">
+      <c r="I31" s="82" t="s">
         <v>283</v>
       </c>
-      <c r="J31" s="91" t="s">
+      <c r="J31" s="82" t="s">
         <v>264</v>
       </c>
-      <c r="K31" s="91">
+      <c r="K31" s="82">
         <v>3</v>
       </c>
-      <c r="L31" s="91">
+      <c r="L31" s="82">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="91" t="s">
+      <c r="M31" s="113"/>
+      <c r="N31" s="113"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="74" t="s">
         <v>300</v>
       </c>
-      <c r="B32" s="95" t="s">
+      <c r="B32" s="78" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="91" t="s">
+      <c r="C32" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D32" s="91" t="s">
+      <c r="D32" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="E32" s="91" t="s">
+      <c r="E32" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="F32" s="91" t="s">
+      <c r="F32" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G32" s="98" t="s">
+      <c r="G32" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="91" t="s">
+      <c r="H32" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="91" t="s">
+      <c r="I32" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="J32" s="91" t="s">
+      <c r="J32" s="74" t="s">
         <v>284</v>
       </c>
-      <c r="K32" s="91">
+      <c r="K32" s="74">
         <v>3</v>
       </c>
-      <c r="L32" s="91">
+      <c r="L32" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="91" t="s">
+    <row r="33" spans="1:14" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="82" t="s">
         <v>301</v>
       </c>
-      <c r="B33" s="95" t="s">
+      <c r="B33" s="109" t="s">
         <v>343</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="D33" s="91" t="s">
+      <c r="D33" s="82" t="s">
         <v>265</v>
       </c>
-      <c r="E33" s="91" t="s">
+      <c r="E33" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="F33" s="91" t="s">
+      <c r="F33" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="G33" s="98" t="s">
+      <c r="G33" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="91" t="s">
+      <c r="H33" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="I33" s="91" t="s">
+      <c r="I33" s="82" t="s">
         <v>276</v>
       </c>
-      <c r="J33" s="91" t="s">
+      <c r="J33" s="82" t="s">
         <v>284</v>
       </c>
-      <c r="K33" s="91">
+      <c r="K33" s="82">
         <v>3</v>
       </c>
-      <c r="L33" s="91">
+      <c r="L33" s="82">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="91" t="s">
+      <c r="M33" s="113"/>
+      <c r="N33" s="113"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B34" s="95" t="s">
+      <c r="B34" s="78" t="s">
         <v>344</v>
       </c>
-      <c r="C34" s="91" t="s">
+      <c r="C34" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="D34" s="91" t="s">
+      <c r="D34" s="74" t="s">
         <v>281</v>
       </c>
-      <c r="E34" s="91" t="s">
+      <c r="E34" s="74" t="s">
         <v>282</v>
       </c>
-      <c r="F34" s="91" t="s">
+      <c r="F34" s="74" t="s">
         <v>272</v>
       </c>
-      <c r="G34" s="98" t="s">
+      <c r="G34" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="H34" s="91" t="s">
+      <c r="H34" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="91" t="s">
+      <c r="I34" s="74" t="s">
         <v>283</v>
       </c>
-      <c r="J34" s="91" t="s">
+      <c r="J34" s="74" t="s">
         <v>284</v>
       </c>
-      <c r="K34" s="91">
+      <c r="K34" s="74">
         <v>3</v>
       </c>
-      <c r="L34" s="91">
+      <c r="L34" s="74">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="91"/>
-      <c r="B38" s="91">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="74"/>
+      <c r="B38" s="74">
         <v>1</v>
       </c>
-      <c r="C38" s="91">
+      <c r="C38" s="74">
         <v>2</v>
       </c>
-      <c r="D38" s="91">
+      <c r="D38" s="74">
         <v>3</v>
       </c>
-      <c r="E38" s="91">
+      <c r="E38" s="74">
         <v>4</v>
       </c>
-      <c r="F38" s="91">
+      <c r="F38" s="74">
         <v>5</v>
       </c>
-      <c r="G38" s="91">
+      <c r="G38" s="74">
         <v>6</v>
       </c>
-      <c r="H38" s="91">
+      <c r="H38" s="74">
         <v>7</v>
       </c>
-      <c r="I38" s="91">
+      <c r="I38" s="74">
         <v>8</v>
       </c>
-      <c r="J38" s="91">
+      <c r="J38" s="74">
         <v>9</v>
       </c>
-      <c r="K38" s="91">
+      <c r="K38" s="74">
         <v>10</v>
       </c>
-      <c r="L38" s="91">
+      <c r="L38" s="74">
         <v>11</v>
       </c>
-      <c r="M38" s="91">
+      <c r="M38" s="74">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="91" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="C39" s="91" t="s">
+      <c r="C39" s="74" t="s">
         <v>256</v>
       </c>
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="E39" s="91" t="s">
+      <c r="E39" s="74" t="s">
         <v>297</v>
       </c>
-      <c r="F39" s="91"/>
-      <c r="G39" s="91"/>
-      <c r="H39" s="91"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="91"/>
-      <c r="L39" s="91"/>
-      <c r="M39" s="91"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="91" t="s">
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="74"/>
+      <c r="M39" s="74"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="C40" s="91" t="s">
+      <c r="C40" s="74" t="s">
         <v>257</v>
       </c>
-      <c r="D40" s="91" t="s">
+      <c r="D40" s="74" t="s">
         <v>285</v>
       </c>
-      <c r="E40" s="91" t="s">
+      <c r="E40" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
-      <c r="I40" s="91"/>
-      <c r="J40" s="91"/>
-      <c r="K40" s="91"/>
-      <c r="L40" s="91"/>
-      <c r="M40" s="91"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="91" t="s">
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="74"/>
+      <c r="L40" s="74"/>
+      <c r="M40" s="74"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="C41" s="91" t="s">
+      <c r="C41" s="74" t="s">
         <v>258</v>
       </c>
-      <c r="D41" s="91" t="s">
+      <c r="D41" s="74" t="s">
         <v>286</v>
       </c>
-      <c r="E41" s="91" t="s">
+      <c r="E41" s="74" t="s">
         <v>299</v>
       </c>
-      <c r="F41" s="91"/>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="91"/>
-      <c r="J41" s="91"/>
-      <c r="K41" s="91"/>
-      <c r="L41" s="91"/>
-      <c r="M41" s="91"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="91" t="s">
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="74"/>
+      <c r="M41" s="74"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="91" t="s">
+      <c r="B42" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="C42" s="91" t="s">
+      <c r="C42" s="74" t="s">
         <v>259</v>
       </c>
-      <c r="D42" s="91" t="s">
+      <c r="D42" s="74" t="s">
         <v>292</v>
       </c>
-      <c r="E42" s="91" t="s">
+      <c r="E42" s="74" t="s">
         <v>300</v>
       </c>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
-      <c r="H42" s="91"/>
-      <c r="I42" s="91"/>
-      <c r="J42" s="91"/>
-      <c r="K42" s="91"/>
-      <c r="L42" s="91"/>
-      <c r="M42" s="91"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="91" t="s">
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="C43" s="91" t="s">
+      <c r="C43" s="74" t="s">
         <v>260</v>
       </c>
-      <c r="D43" s="91" t="s">
+      <c r="D43" s="74" t="s">
         <v>293</v>
       </c>
-      <c r="E43" s="91" t="s">
+      <c r="E43" s="74" t="s">
         <v>301</v>
       </c>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="91"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91"/>
-      <c r="K43" s="91"/>
-      <c r="L43" s="91"/>
-      <c r="M43" s="91"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="91" t="s">
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="74"/>
+      <c r="M43" s="74"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="B44" s="91" t="s">
+      <c r="B44" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="91" t="s">
+      <c r="C44" s="74" t="s">
         <v>261</v>
       </c>
-      <c r="D44" s="91" t="s">
+      <c r="D44" s="74" t="s">
         <v>294</v>
       </c>
-      <c r="E44" s="91" t="s">
+      <c r="E44" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="F44" s="91"/>
-      <c r="G44" s="91"/>
-      <c r="H44" s="91"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="91"/>
-      <c r="K44" s="91"/>
-      <c r="L44" s="91"/>
-      <c r="M44" s="91"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="91" t="s">
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="74"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="91" t="s">
+      <c r="C45" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="D45" s="91" t="s">
+      <c r="D45" s="74" t="s">
         <v>295</v>
       </c>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="91"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="91"/>
-      <c r="M45" s="91"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="91" t="s">
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="74"/>
+      <c r="M45" s="74"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="91" t="s">
+      <c r="B46" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="C46" s="91" t="s">
+      <c r="C46" s="74" t="s">
         <v>279</v>
       </c>
-      <c r="D46" s="91" t="s">
+      <c r="D46" s="74" t="s">
         <v>296</v>
       </c>
-      <c r="E46" s="91"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="91"/>
-      <c r="H46" s="91"/>
-      <c r="I46" s="91"/>
-      <c r="J46" s="91"/>
-      <c r="K46" s="91"/>
-      <c r="L46" s="91"/>
-      <c r="M46" s="91"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="74"/>
+      <c r="M46" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:M1"/>
+    <mergeCell ref="C2:F2"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V3V4 test run pipeline post Wesley chat
</commit_message>
<xml_diff>
--- a/Lab-work/V3V4_16S_March2020.xlsx
+++ b/Lab-work/V3V4_16S_March2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/EmmaStrand_Notebook/Lab-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBACB3FF-0890-1D4A-A94D-E453DF3A83A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7AE716-DB2A-6F4F-8CED-0D604FA463D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36280" yWindow="1380" windowWidth="32520" windowHeight="19560" firstSheet="4" activeTab="8" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
+    <workbookView xWindow="5500" yWindow="460" windowWidth="28100" windowHeight="19560" firstSheet="4" activeTab="8" xr2:uid="{EBBF8BB8-3757-E140-A0F6-9E178C0E96EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Primer choice" sheetId="1" r:id="rId1"/>
@@ -1707,6 +1707,19 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1761,19 +1774,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2106,12 +2106,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2224,10 +2224,10 @@
       <c r="C9" s="60"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="107" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="98"/>
+      <c r="B13" s="107"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -2288,10 +2288,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="98" t="s">
+      <c r="A32" s="107" t="s">
         <v>189</v>
       </c>
-      <c r="B32" s="98"/>
+      <c r="B32" s="107"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
@@ -2386,20 +2386,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="97" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="97" t="s">
         <v>347</v>
       </c>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-    </row>
-    <row r="4" spans="1:15" s="116" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+    </row>
+    <row r="4" spans="1:15" s="98" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="84" t="s">
         <v>345</v>
       </c>
@@ -2626,9 +2626,9 @@
       <c r="L9" s="86" t="s">
         <v>367</v>
       </c>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
+      <c r="O9" s="99"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="85" t="s">
@@ -2667,9 +2667,9 @@
       <c r="L10" s="86" t="s">
         <v>367</v>
       </c>
-      <c r="M10" s="118"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="118"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="101"/>
+      <c r="O10" s="100"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="85" t="s">
@@ -2708,9 +2708,9 @@
       <c r="L11" s="86" t="s">
         <v>367</v>
       </c>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="118"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="100"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="85" t="s">
@@ -2749,9 +2749,9 @@
       <c r="L12" s="86" t="s">
         <v>367</v>
       </c>
-      <c r="M12" s="118"/>
-      <c r="N12" s="120"/>
-      <c r="O12" s="118"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="100"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="85" t="s">
@@ -2790,9 +2790,9 @@
       <c r="L13" s="86" t="s">
         <v>367</v>
       </c>
-      <c r="M13" s="118"/>
-      <c r="N13" s="120"/>
-      <c r="O13" s="120"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="85" t="s">
@@ -3593,7 +3593,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="121" t="s">
+      <c r="A36" s="103" t="s">
         <v>369</v>
       </c>
     </row>
@@ -3611,7 +3611,7 @@
       <c r="E37" s="81">
         <v>4</v>
       </c>
-      <c r="F37" s="122"/>
+      <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="81" t="s">
@@ -3629,11 +3629,11 @@
       <c r="E38" s="81" t="s">
         <v>297</v>
       </c>
-      <c r="F38" s="122"/>
-      <c r="G38" s="117"/>
-      <c r="H38" s="117"/>
-      <c r="I38" s="117"/>
-      <c r="J38" s="117"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="99"/>
+      <c r="I38" s="99"/>
+      <c r="J38" s="99"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="81" t="s">
@@ -3651,11 +3651,11 @@
       <c r="E39" s="81" t="s">
         <v>298</v>
       </c>
-      <c r="F39" s="122"/>
-      <c r="G39" s="123"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="119"/>
-      <c r="J39" s="118"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="105"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="100"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="81" t="s">
@@ -3673,11 +3673,11 @@
       <c r="E40" s="81" t="s">
         <v>299</v>
       </c>
-      <c r="F40" s="122"/>
-      <c r="G40" s="123"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="118"/>
-      <c r="J40" s="118"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="105"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="81" t="s">
@@ -3695,11 +3695,11 @@
       <c r="E41" s="81" t="s">
         <v>300</v>
       </c>
-      <c r="F41" s="122"/>
-      <c r="G41" s="123"/>
-      <c r="H41" s="118"/>
-      <c r="I41" s="120"/>
-      <c r="J41" s="118"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="105"/>
+      <c r="H41" s="100"/>
+      <c r="I41" s="102"/>
+      <c r="J41" s="100"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="81" t="s">
@@ -3717,11 +3717,11 @@
       <c r="E42" s="81" t="s">
         <v>301</v>
       </c>
-      <c r="F42" s="122"/>
-      <c r="G42" s="123"/>
-      <c r="H42" s="118"/>
-      <c r="I42" s="120"/>
-      <c r="J42" s="120"/>
+      <c r="F42" s="104"/>
+      <c r="G42" s="105"/>
+      <c r="H42" s="100"/>
+      <c r="I42" s="102"/>
+      <c r="J42" s="102"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="81" t="s">
@@ -3739,7 +3739,7 @@
       <c r="E43" s="81" t="s">
         <v>302</v>
       </c>
-      <c r="F43" s="122"/>
+      <c r="F43" s="104"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="81" t="s">
@@ -3755,7 +3755,7 @@
         <v>295</v>
       </c>
       <c r="E44" s="81"/>
-      <c r="F44" s="122"/>
+      <c r="F44" s="104"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="81" t="s">
@@ -3771,7 +3771,7 @@
         <v>296</v>
       </c>
       <c r="E45" s="81"/>
-      <c r="F45" s="122"/>
+      <c r="F45" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3825,7 +3825,7 @@
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="108" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3836,7 +3836,7 @@
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="108"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -3845,7 +3845,7 @@
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="99"/>
+      <c r="C5" s="108"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -3891,20 +3891,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
     </row>
     <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -3935,16 +3935,16 @@
         <v>85</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="102" t="s">
+      <c r="K3" s="111" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="102"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -4361,12 +4361,12 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="101" t="s">
+      <c r="A16" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
       <c r="K16" s="5">
         <v>1</v>
       </c>
@@ -4515,12 +4515,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
       <c r="K24" s="5">
         <v>1</v>
       </c>
@@ -4724,32 +4724,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
@@ -5110,12 +5110,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -5165,12 +5165,12 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -5266,16 +5266,16 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="102" t="s">
+      <c r="A35" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="102"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="102"/>
-      <c r="H35" s="102"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="111"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
@@ -5470,17 +5470,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -5764,12 +5764,12 @@
       <c r="M13" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
@@ -6193,39 +6193,39 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="107"/>
-      <c r="F33" s="107"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="107"/>
-      <c r="I33" s="108"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="116"/>
+      <c r="H33" s="116"/>
+      <c r="I33" s="117"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="109" t="s">
+      <c r="B34" s="118" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="111"/>
+      <c r="C34" s="119"/>
+      <c r="D34" s="119"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="119"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="120"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="101" t="s">
+      <c r="A37" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="101"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
+      <c r="B37" s="110"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="110"/>
       <c r="F37" s="55" t="s">
         <v>159</v>
       </c>
@@ -6371,29 +6371,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="121" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="118" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="111"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="120"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -6651,12 +6651,12 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="101" t="s">
+      <c r="A27" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="101"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
       <c r="F27" s="55" t="s">
         <v>159</v>
       </c>
@@ -6804,26 +6804,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="122" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -7219,17 +7219,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="121" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -7542,7 +7542,7 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7565,21 +7565,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="121" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
       <c r="N1" s="74"/>
       <c r="O1" s="74"/>
       <c r="P1" s="74"/>
@@ -7589,10 +7589,10 @@
       <c r="A2" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
     </row>
     <row r="4" spans="1:17" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="76" t="s">

</xml_diff>